<commit_message>
Updated models and added those for reduced supplementary skills
</commit_message>
<xml_diff>
--- a/data/new_posteriors/elementary_skills/complex_model/noleak/questions-skill-model2b_noleak.xlsx
+++ b/data/new_posteriors/elementary_skills/complex_model/noleak/questions-skill-model2b_noleak.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgia/repositories/virtual-CAT-itas/data/CAT_COMMANDS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgia/repositories/virtual-CAT-itas/data/new_posteriors/elementary_skills/complex_model/noleak/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2224C9CF-B54F-3C40-9889-426434732751}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB920AD-6BF3-C045-A0A6-665BDCF45159}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10920" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{3D5E00E8-EA45-C34D-85AA-17AD78DA61C2}"/>
+    <workbookView xWindow="120" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{3D5E00E8-EA45-C34D-85AA-17AD78DA61C2}"/>
   </bookViews>
   <sheets>
     <sheet name="question-skills-complex" sheetId="17" r:id="rId1"/>
@@ -685,9 +685,6 @@
     <xf numFmtId="2" fontId="2" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -695,6 +692,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1037,11 +1037,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85B7A501-D8DC-5145-BD21-F7991AE9B547}">
   <dimension ref="A1:NI588"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B461" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="88" workbookViewId="0">
+      <pane xSplit="2" ySplit="4" topLeftCell="U435" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="L499" sqref="L499"/>
+      <selection pane="bottomRight" activeCell="AE482" sqref="AE482:AF484"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1178,7 +1178,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:373" s="7" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:373" s="7" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" s="53"/>
       <c r="B3" s="53"/>
       <c r="C3" s="53"/>
@@ -2221,7 +2221,7 @@
       <c r="NI5"/>
     </row>
     <row r="6" spans="1:373" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="46"/>
+      <c r="A6" s="49"/>
       <c r="B6" s="13">
         <v>2</v>
       </c>
@@ -2351,7 +2351,7 @@
       </c>
     </row>
     <row r="7" spans="1:373" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="46"/>
+      <c r="A7" s="49"/>
       <c r="B7" s="13">
         <v>3</v>
       </c>
@@ -2481,7 +2481,7 @@
       </c>
     </row>
     <row r="8" spans="1:373" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="46"/>
+      <c r="A8" s="49"/>
       <c r="B8" s="13">
         <v>4</v>
       </c>
@@ -2611,7 +2611,7 @@
       </c>
     </row>
     <row r="9" spans="1:373" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="46"/>
+      <c r="A9" s="49"/>
       <c r="B9" s="13">
         <v>5</v>
       </c>
@@ -2741,7 +2741,7 @@
       </c>
     </row>
     <row r="10" spans="1:373" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="46"/>
+      <c r="A10" s="49"/>
       <c r="B10" s="13">
         <v>6</v>
       </c>
@@ -2871,7 +2871,7 @@
       </c>
     </row>
     <row r="11" spans="1:373" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="46"/>
+      <c r="A11" s="49"/>
       <c r="B11" s="13">
         <v>7</v>
       </c>
@@ -3001,7 +3001,7 @@
       </c>
     </row>
     <row r="12" spans="1:373" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="46"/>
+      <c r="A12" s="49"/>
       <c r="B12" s="13">
         <v>8</v>
       </c>
@@ -3131,7 +3131,7 @@
       </c>
     </row>
     <row r="13" spans="1:373" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="46"/>
+      <c r="A13" s="49"/>
       <c r="B13" s="13">
         <v>9</v>
       </c>
@@ -3261,7 +3261,7 @@
       </c>
     </row>
     <row r="14" spans="1:373" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="46"/>
+      <c r="A14" s="49"/>
       <c r="B14" s="13">
         <v>10</v>
       </c>
@@ -3391,7 +3391,7 @@
       </c>
     </row>
     <row r="15" spans="1:373" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="46"/>
+      <c r="A15" s="49"/>
       <c r="B15" s="13">
         <v>11</v>
       </c>
@@ -3521,7 +3521,7 @@
       </c>
     </row>
     <row r="16" spans="1:373" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="46"/>
+      <c r="A16" s="49"/>
       <c r="B16" s="13">
         <v>12</v>
       </c>
@@ -3651,7 +3651,7 @@
       </c>
     </row>
     <row r="17" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="46"/>
+      <c r="A17" s="49"/>
       <c r="B17" s="13">
         <v>13</v>
       </c>
@@ -3781,7 +3781,7 @@
       </c>
     </row>
     <row r="18" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="46"/>
+      <c r="A18" s="49"/>
       <c r="B18" s="13">
         <v>14</v>
       </c>
@@ -3911,7 +3911,7 @@
       </c>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="46"/>
+      <c r="A19" s="49"/>
       <c r="B19" s="13">
         <v>15</v>
       </c>
@@ -4041,7 +4041,7 @@
       </c>
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="46"/>
+      <c r="A20" s="49"/>
       <c r="B20" s="13">
         <v>16</v>
       </c>
@@ -4171,7 +4171,7 @@
       </c>
     </row>
     <row r="21" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="46"/>
+      <c r="A21" s="49"/>
       <c r="B21" s="13">
         <v>17</v>
       </c>
@@ -4301,7 +4301,7 @@
       </c>
     </row>
     <row r="22" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="46"/>
+      <c r="A22" s="49"/>
       <c r="B22" s="13">
         <v>18</v>
       </c>
@@ -4431,7 +4431,7 @@
       </c>
     </row>
     <row r="23" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="46"/>
+      <c r="A23" s="49"/>
       <c r="B23" s="13">
         <v>19</v>
       </c>
@@ -4561,7 +4561,7 @@
       </c>
     </row>
     <row r="24" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="46"/>
+      <c r="A24" s="49"/>
       <c r="B24" s="13">
         <v>20</v>
       </c>
@@ -4691,7 +4691,7 @@
       </c>
     </row>
     <row r="25" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="46"/>
+      <c r="A25" s="49"/>
       <c r="B25" s="13">
         <v>21</v>
       </c>
@@ -4821,7 +4821,7 @@
       </c>
     </row>
     <row r="26" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="46"/>
+      <c r="A26" s="49"/>
       <c r="B26" s="13">
         <v>22</v>
       </c>
@@ -4951,7 +4951,7 @@
       </c>
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="46"/>
+      <c r="A27" s="49"/>
       <c r="B27" s="13">
         <v>23</v>
       </c>
@@ -5081,7 +5081,7 @@
       </c>
     </row>
     <row r="28" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="46"/>
+      <c r="A28" s="49"/>
       <c r="B28" s="13">
         <v>24</v>
       </c>
@@ -5211,7 +5211,7 @@
       </c>
     </row>
     <row r="29" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="46"/>
+      <c r="A29" s="49"/>
       <c r="B29" s="13">
         <v>25</v>
       </c>
@@ -5341,7 +5341,7 @@
       </c>
     </row>
     <row r="30" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="46"/>
+      <c r="A30" s="49"/>
       <c r="B30" s="13">
         <v>26</v>
       </c>
@@ -5471,7 +5471,7 @@
       </c>
     </row>
     <row r="31" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="46"/>
+      <c r="A31" s="49"/>
       <c r="B31" s="13">
         <v>27</v>
       </c>
@@ -5601,7 +5601,7 @@
       </c>
     </row>
     <row r="32" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="46"/>
+      <c r="A32" s="49"/>
       <c r="B32" s="13">
         <v>28</v>
       </c>
@@ -5731,7 +5731,7 @@
       </c>
     </row>
     <row r="33" spans="1:373" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="46"/>
+      <c r="A33" s="49"/>
       <c r="B33" s="13">
         <v>29</v>
       </c>
@@ -5861,7 +5861,7 @@
       </c>
     </row>
     <row r="34" spans="1:373" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="46"/>
+      <c r="A34" s="49"/>
       <c r="B34" s="13">
         <v>30</v>
       </c>
@@ -5991,7 +5991,7 @@
       </c>
     </row>
     <row r="35" spans="1:373" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="46"/>
+      <c r="A35" s="49"/>
       <c r="B35" s="13">
         <v>31</v>
       </c>
@@ -6121,7 +6121,7 @@
       </c>
     </row>
     <row r="36" spans="1:373" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="46"/>
+      <c r="A36" s="49"/>
       <c r="B36" s="16">
         <v>32</v>
       </c>
@@ -6580,7 +6580,7 @@
       <c r="NI36" s="2"/>
     </row>
     <row r="37" spans="1:373" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="46"/>
+      <c r="A37" s="49"/>
       <c r="B37" s="13">
         <v>33</v>
       </c>
@@ -6709,7 +6709,7 @@
       </c>
     </row>
     <row r="38" spans="1:373" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="46"/>
+      <c r="A38" s="49"/>
       <c r="B38" s="13">
         <v>34</v>
       </c>
@@ -6717,7 +6717,7 @@
         <v>54</v>
       </c>
       <c r="D38" s="3">
-        <v>0.5</v>
+        <v>0.65</v>
       </c>
       <c r="E38" s="4">
         <v>0</v>
@@ -6838,7 +6838,7 @@
       </c>
     </row>
     <row r="39" spans="1:373" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="46"/>
+      <c r="A39" s="49"/>
       <c r="B39" s="13">
         <v>35</v>
       </c>
@@ -6967,7 +6967,7 @@
       </c>
     </row>
     <row r="40" spans="1:373" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="46"/>
+      <c r="A40" s="49"/>
       <c r="B40" s="13">
         <v>36</v>
       </c>
@@ -7096,7 +7096,7 @@
       </c>
     </row>
     <row r="41" spans="1:373" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="46"/>
+      <c r="A41" s="49"/>
       <c r="B41" s="13">
         <v>37</v>
       </c>
@@ -7225,7 +7225,7 @@
       </c>
     </row>
     <row r="42" spans="1:373" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="46"/>
+      <c r="A42" s="49"/>
       <c r="B42" s="13">
         <v>38</v>
       </c>
@@ -7354,7 +7354,7 @@
       </c>
     </row>
     <row r="43" spans="1:373" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="46"/>
+      <c r="A43" s="49"/>
       <c r="B43" s="13">
         <v>39</v>
       </c>
@@ -7483,7 +7483,7 @@
       </c>
     </row>
     <row r="44" spans="1:373" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="46"/>
+      <c r="A44" s="49"/>
       <c r="B44" s="13">
         <v>40</v>
       </c>
@@ -7942,7 +7942,7 @@
       <c r="NI44" s="2"/>
     </row>
     <row r="45" spans="1:373" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="47">
+      <c r="A45" s="46">
         <v>2</v>
       </c>
       <c r="B45" s="16">
@@ -8404,7 +8404,7 @@
       <c r="NI45"/>
     </row>
     <row r="46" spans="1:373" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="48"/>
+      <c r="A46" s="47"/>
       <c r="B46" s="13">
         <v>2</v>
       </c>
@@ -8534,7 +8534,7 @@
       </c>
     </row>
     <row r="47" spans="1:373" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="48"/>
+      <c r="A47" s="47"/>
       <c r="B47" s="13">
         <v>3</v>
       </c>
@@ -8664,7 +8664,7 @@
       </c>
     </row>
     <row r="48" spans="1:373" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="48"/>
+      <c r="A48" s="47"/>
       <c r="B48" s="13">
         <v>4</v>
       </c>
@@ -8794,7 +8794,7 @@
       </c>
     </row>
     <row r="49" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="48"/>
+      <c r="A49" s="47"/>
       <c r="B49" s="13">
         <v>5</v>
       </c>
@@ -8924,7 +8924,7 @@
       </c>
     </row>
     <row r="50" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="48"/>
+      <c r="A50" s="47"/>
       <c r="B50" s="13">
         <v>6</v>
       </c>
@@ -9054,7 +9054,7 @@
       </c>
     </row>
     <row r="51" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="48"/>
+      <c r="A51" s="47"/>
       <c r="B51" s="13">
         <v>7</v>
       </c>
@@ -9184,7 +9184,7 @@
       </c>
     </row>
     <row r="52" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="48"/>
+      <c r="A52" s="47"/>
       <c r="B52" s="13">
         <v>8</v>
       </c>
@@ -9314,7 +9314,7 @@
       </c>
     </row>
     <row r="53" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="48"/>
+      <c r="A53" s="47"/>
       <c r="B53" s="13">
         <v>9</v>
       </c>
@@ -9444,7 +9444,7 @@
       </c>
     </row>
     <row r="54" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="48"/>
+      <c r="A54" s="47"/>
       <c r="B54" s="13">
         <v>10</v>
       </c>
@@ -9574,7 +9574,7 @@
       </c>
     </row>
     <row r="55" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="48"/>
+      <c r="A55" s="47"/>
       <c r="B55" s="13">
         <v>11</v>
       </c>
@@ -9704,7 +9704,7 @@
       </c>
     </row>
     <row r="56" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="48"/>
+      <c r="A56" s="47"/>
       <c r="B56" s="13">
         <v>12</v>
       </c>
@@ -9834,7 +9834,7 @@
       </c>
     </row>
     <row r="57" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="48"/>
+      <c r="A57" s="47"/>
       <c r="B57" s="13">
         <v>13</v>
       </c>
@@ -9964,7 +9964,7 @@
       </c>
     </row>
     <row r="58" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="48"/>
+      <c r="A58" s="47"/>
       <c r="B58" s="13">
         <v>14</v>
       </c>
@@ -10094,7 +10094,7 @@
       </c>
     </row>
     <row r="59" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="48"/>
+      <c r="A59" s="47"/>
       <c r="B59" s="13">
         <v>15</v>
       </c>
@@ -10224,7 +10224,7 @@
       </c>
     </row>
     <row r="60" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="48"/>
+      <c r="A60" s="47"/>
       <c r="B60" s="13">
         <v>16</v>
       </c>
@@ -10354,7 +10354,7 @@
       </c>
     </row>
     <row r="61" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="48"/>
+      <c r="A61" s="47"/>
       <c r="B61" s="13">
         <v>17</v>
       </c>
@@ -10484,7 +10484,7 @@
       </c>
     </row>
     <row r="62" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="48"/>
+      <c r="A62" s="47"/>
       <c r="B62" s="13">
         <v>18</v>
       </c>
@@ -10614,7 +10614,7 @@
       </c>
     </row>
     <row r="63" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="48"/>
+      <c r="A63" s="47"/>
       <c r="B63" s="13">
         <v>19</v>
       </c>
@@ -10744,7 +10744,7 @@
       </c>
     </row>
     <row r="64" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="48"/>
+      <c r="A64" s="47"/>
       <c r="B64" s="13">
         <v>20</v>
       </c>
@@ -10874,7 +10874,7 @@
       </c>
     </row>
     <row r="65" spans="1:373" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="48"/>
+      <c r="A65" s="47"/>
       <c r="B65" s="13">
         <v>21</v>
       </c>
@@ -11004,7 +11004,7 @@
       </c>
     </row>
     <row r="66" spans="1:373" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="48"/>
+      <c r="A66" s="47"/>
       <c r="B66" s="13">
         <v>22</v>
       </c>
@@ -11134,7 +11134,7 @@
       </c>
     </row>
     <row r="67" spans="1:373" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="48"/>
+      <c r="A67" s="47"/>
       <c r="B67" s="13">
         <v>23</v>
       </c>
@@ -11264,7 +11264,7 @@
       </c>
     </row>
     <row r="68" spans="1:373" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="48"/>
+      <c r="A68" s="47"/>
       <c r="B68" s="13">
         <v>24</v>
       </c>
@@ -11394,7 +11394,7 @@
       </c>
     </row>
     <row r="69" spans="1:373" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="48"/>
+      <c r="A69" s="47"/>
       <c r="B69" s="13">
         <v>25</v>
       </c>
@@ -11524,7 +11524,7 @@
       </c>
     </row>
     <row r="70" spans="1:373" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="48"/>
+      <c r="A70" s="47"/>
       <c r="B70" s="13">
         <v>26</v>
       </c>
@@ -11654,7 +11654,7 @@
       </c>
     </row>
     <row r="71" spans="1:373" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="48"/>
+      <c r="A71" s="47"/>
       <c r="B71" s="13">
         <v>27</v>
       </c>
@@ -11784,7 +11784,7 @@
       </c>
     </row>
     <row r="72" spans="1:373" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="48"/>
+      <c r="A72" s="47"/>
       <c r="B72" s="13">
         <v>28</v>
       </c>
@@ -11914,7 +11914,7 @@
       </c>
     </row>
     <row r="73" spans="1:373" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="48"/>
+      <c r="A73" s="47"/>
       <c r="B73" s="13">
         <v>29</v>
       </c>
@@ -12044,7 +12044,7 @@
       </c>
     </row>
     <row r="74" spans="1:373" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="48"/>
+      <c r="A74" s="47"/>
       <c r="B74" s="13">
         <v>30</v>
       </c>
@@ -12174,7 +12174,7 @@
       </c>
     </row>
     <row r="75" spans="1:373" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="48"/>
+      <c r="A75" s="47"/>
       <c r="B75" s="13">
         <v>31</v>
       </c>
@@ -12304,7 +12304,7 @@
       </c>
     </row>
     <row r="76" spans="1:373" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="48"/>
+      <c r="A76" s="47"/>
       <c r="B76" s="16">
         <v>32</v>
       </c>
@@ -12763,7 +12763,7 @@
       <c r="NI76" s="2"/>
     </row>
     <row r="77" spans="1:373" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="48"/>
+      <c r="A77" s="47"/>
       <c r="B77" s="13">
         <v>33</v>
       </c>
@@ -12892,7 +12892,7 @@
       </c>
     </row>
     <row r="78" spans="1:373" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="48"/>
+      <c r="A78" s="47"/>
       <c r="B78" s="13">
         <v>34</v>
       </c>
@@ -12900,7 +12900,7 @@
         <v>54</v>
       </c>
       <c r="D78" s="42">
-        <v>0.5</v>
+        <v>0.65</v>
       </c>
       <c r="E78" s="4">
         <v>0</v>
@@ -13021,7 +13021,7 @@
       </c>
     </row>
     <row r="79" spans="1:373" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="48"/>
+      <c r="A79" s="47"/>
       <c r="B79" s="13">
         <v>35</v>
       </c>
@@ -13150,7 +13150,7 @@
       </c>
     </row>
     <row r="80" spans="1:373" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="48"/>
+      <c r="A80" s="47"/>
       <c r="B80" s="13">
         <v>36</v>
       </c>
@@ -13279,7 +13279,7 @@
       </c>
     </row>
     <row r="81" spans="1:373" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="48"/>
+      <c r="A81" s="47"/>
       <c r="B81" s="13">
         <v>37</v>
       </c>
@@ -13408,7 +13408,7 @@
       </c>
     </row>
     <row r="82" spans="1:373" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="48"/>
+      <c r="A82" s="47"/>
       <c r="B82" s="13">
         <v>38</v>
       </c>
@@ -13537,7 +13537,7 @@
       </c>
     </row>
     <row r="83" spans="1:373" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="48"/>
+      <c r="A83" s="47"/>
       <c r="B83" s="13">
         <v>39</v>
       </c>
@@ -13666,7 +13666,7 @@
       </c>
     </row>
     <row r="84" spans="1:373" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="49"/>
+      <c r="A84" s="48"/>
       <c r="B84" s="20">
         <v>40</v>
       </c>
@@ -14125,7 +14125,7 @@
       <c r="NI84" s="2"/>
     </row>
     <row r="85" spans="1:373" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="46">
+      <c r="A85" s="49">
         <v>3</v>
       </c>
       <c r="B85" s="13">
@@ -14587,7 +14587,7 @@
       <c r="NI85"/>
     </row>
     <row r="86" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A86" s="46"/>
+      <c r="A86" s="49"/>
       <c r="B86" s="13">
         <v>2</v>
       </c>
@@ -14717,7 +14717,7 @@
       </c>
     </row>
     <row r="87" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A87" s="46"/>
+      <c r="A87" s="49"/>
       <c r="B87" s="13">
         <v>3</v>
       </c>
@@ -14847,7 +14847,7 @@
       </c>
     </row>
     <row r="88" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A88" s="46"/>
+      <c r="A88" s="49"/>
       <c r="B88" s="13">
         <v>4</v>
       </c>
@@ -14977,7 +14977,7 @@
       </c>
     </row>
     <row r="89" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A89" s="46"/>
+      <c r="A89" s="49"/>
       <c r="B89" s="13">
         <v>5</v>
       </c>
@@ -15107,7 +15107,7 @@
       </c>
     </row>
     <row r="90" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A90" s="46"/>
+      <c r="A90" s="49"/>
       <c r="B90" s="13">
         <v>6</v>
       </c>
@@ -15237,7 +15237,7 @@
       </c>
     </row>
     <row r="91" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A91" s="46"/>
+      <c r="A91" s="49"/>
       <c r="B91" s="13">
         <v>7</v>
       </c>
@@ -15367,7 +15367,7 @@
       </c>
     </row>
     <row r="92" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A92" s="46"/>
+      <c r="A92" s="49"/>
       <c r="B92" s="13">
         <v>8</v>
       </c>
@@ -15497,7 +15497,7 @@
       </c>
     </row>
     <row r="93" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A93" s="46"/>
+      <c r="A93" s="49"/>
       <c r="B93" s="13">
         <v>9</v>
       </c>
@@ -15627,7 +15627,7 @@
       </c>
     </row>
     <row r="94" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A94" s="46"/>
+      <c r="A94" s="49"/>
       <c r="B94" s="13">
         <v>10</v>
       </c>
@@ -15757,7 +15757,7 @@
       </c>
     </row>
     <row r="95" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A95" s="46"/>
+      <c r="A95" s="49"/>
       <c r="B95" s="13">
         <v>11</v>
       </c>
@@ -15887,7 +15887,7 @@
       </c>
     </row>
     <row r="96" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A96" s="46"/>
+      <c r="A96" s="49"/>
       <c r="B96" s="13">
         <v>12</v>
       </c>
@@ -16017,7 +16017,7 @@
       </c>
     </row>
     <row r="97" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A97" s="46"/>
+      <c r="A97" s="49"/>
       <c r="B97" s="13">
         <v>13</v>
       </c>
@@ -16147,7 +16147,7 @@
       </c>
     </row>
     <row r="98" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A98" s="46"/>
+      <c r="A98" s="49"/>
       <c r="B98" s="13">
         <v>14</v>
       </c>
@@ -16277,7 +16277,7 @@
       </c>
     </row>
     <row r="99" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A99" s="46"/>
+      <c r="A99" s="49"/>
       <c r="B99" s="13">
         <v>15</v>
       </c>
@@ -16407,7 +16407,7 @@
       </c>
     </row>
     <row r="100" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A100" s="46"/>
+      <c r="A100" s="49"/>
       <c r="B100" s="13">
         <v>16</v>
       </c>
@@ -16537,7 +16537,7 @@
       </c>
     </row>
     <row r="101" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A101" s="46"/>
+      <c r="A101" s="49"/>
       <c r="B101" s="13">
         <v>17</v>
       </c>
@@ -16667,7 +16667,7 @@
       </c>
     </row>
     <row r="102" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A102" s="46"/>
+      <c r="A102" s="49"/>
       <c r="B102" s="13">
         <v>18</v>
       </c>
@@ -16797,7 +16797,7 @@
       </c>
     </row>
     <row r="103" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A103" s="46"/>
+      <c r="A103" s="49"/>
       <c r="B103" s="13">
         <v>19</v>
       </c>
@@ -16927,7 +16927,7 @@
       </c>
     </row>
     <row r="104" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A104" s="46"/>
+      <c r="A104" s="49"/>
       <c r="B104" s="13">
         <v>20</v>
       </c>
@@ -17057,7 +17057,7 @@
       </c>
     </row>
     <row r="105" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A105" s="46"/>
+      <c r="A105" s="49"/>
       <c r="B105" s="13">
         <v>21</v>
       </c>
@@ -17187,7 +17187,7 @@
       </c>
     </row>
     <row r="106" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A106" s="46"/>
+      <c r="A106" s="49"/>
       <c r="B106" s="13">
         <v>22</v>
       </c>
@@ -17317,7 +17317,7 @@
       </c>
     </row>
     <row r="107" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A107" s="46"/>
+      <c r="A107" s="49"/>
       <c r="B107" s="13">
         <v>23</v>
       </c>
@@ -17447,7 +17447,7 @@
       </c>
     </row>
     <row r="108" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A108" s="46"/>
+      <c r="A108" s="49"/>
       <c r="B108" s="13">
         <v>24</v>
       </c>
@@ -17577,7 +17577,7 @@
       </c>
     </row>
     <row r="109" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A109" s="46"/>
+      <c r="A109" s="49"/>
       <c r="B109" s="13">
         <v>25</v>
       </c>
@@ -17707,7 +17707,7 @@
       </c>
     </row>
     <row r="110" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A110" s="46"/>
+      <c r="A110" s="49"/>
       <c r="B110" s="13">
         <v>26</v>
       </c>
@@ -17837,7 +17837,7 @@
       </c>
     </row>
     <row r="111" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A111" s="46"/>
+      <c r="A111" s="49"/>
       <c r="B111" s="13">
         <v>27</v>
       </c>
@@ -17967,7 +17967,7 @@
       </c>
     </row>
     <row r="112" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A112" s="46"/>
+      <c r="A112" s="49"/>
       <c r="B112" s="13">
         <v>28</v>
       </c>
@@ -18097,7 +18097,7 @@
       </c>
     </row>
     <row r="113" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A113" s="46"/>
+      <c r="A113" s="49"/>
       <c r="B113" s="13">
         <v>29</v>
       </c>
@@ -18227,7 +18227,7 @@
       </c>
     </row>
     <row r="114" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A114" s="46"/>
+      <c r="A114" s="49"/>
       <c r="B114" s="13">
         <v>30</v>
       </c>
@@ -18357,7 +18357,7 @@
       </c>
     </row>
     <row r="115" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A115" s="46"/>
+      <c r="A115" s="49"/>
       <c r="B115" s="13">
         <v>31</v>
       </c>
@@ -18487,7 +18487,7 @@
       </c>
     </row>
     <row r="116" spans="1:373" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="46"/>
+      <c r="A116" s="49"/>
       <c r="B116" s="16">
         <v>32</v>
       </c>
@@ -18946,7 +18946,7 @@
       <c r="NI116" s="2"/>
     </row>
     <row r="117" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A117" s="46"/>
+      <c r="A117" s="49"/>
       <c r="B117" s="13">
         <v>33</v>
       </c>
@@ -19075,7 +19075,7 @@
       </c>
     </row>
     <row r="118" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A118" s="46"/>
+      <c r="A118" s="49"/>
       <c r="B118" s="13">
         <v>34</v>
       </c>
@@ -19083,7 +19083,7 @@
         <v>54</v>
       </c>
       <c r="D118" s="37">
-        <v>0.45</v>
+        <v>0.6</v>
       </c>
       <c r="E118" s="4">
         <v>0</v>
@@ -19204,7 +19204,7 @@
       </c>
     </row>
     <row r="119" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A119" s="46"/>
+      <c r="A119" s="49"/>
       <c r="B119" s="13">
         <v>35</v>
       </c>
@@ -19333,7 +19333,7 @@
       </c>
     </row>
     <row r="120" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A120" s="46"/>
+      <c r="A120" s="49"/>
       <c r="B120" s="13">
         <v>36</v>
       </c>
@@ -19462,7 +19462,7 @@
       </c>
     </row>
     <row r="121" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A121" s="46"/>
+      <c r="A121" s="49"/>
       <c r="B121" s="13">
         <v>37</v>
       </c>
@@ -19591,7 +19591,7 @@
       </c>
     </row>
     <row r="122" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A122" s="46"/>
+      <c r="A122" s="49"/>
       <c r="B122" s="13">
         <v>38</v>
       </c>
@@ -19720,7 +19720,7 @@
       </c>
     </row>
     <row r="123" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A123" s="46"/>
+      <c r="A123" s="49"/>
       <c r="B123" s="13">
         <v>39</v>
       </c>
@@ -19849,7 +19849,7 @@
       </c>
     </row>
     <row r="124" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A124" s="46"/>
+      <c r="A124" s="49"/>
       <c r="B124" s="13">
         <v>40</v>
       </c>
@@ -19978,7 +19978,7 @@
       </c>
     </row>
     <row r="125" spans="1:373" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="47">
+      <c r="A125" s="46">
         <v>4</v>
       </c>
       <c r="B125" s="16">
@@ -20440,7 +20440,7 @@
       <c r="NI125"/>
     </row>
     <row r="126" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A126" s="48"/>
+      <c r="A126" s="47"/>
       <c r="B126" s="13">
         <v>2</v>
       </c>
@@ -20570,7 +20570,7 @@
       </c>
     </row>
     <row r="127" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A127" s="48"/>
+      <c r="A127" s="47"/>
       <c r="B127" s="13">
         <v>3</v>
       </c>
@@ -20700,7 +20700,7 @@
       </c>
     </row>
     <row r="128" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A128" s="48"/>
+      <c r="A128" s="47"/>
       <c r="B128" s="13">
         <v>4</v>
       </c>
@@ -20830,7 +20830,7 @@
       </c>
     </row>
     <row r="129" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A129" s="48"/>
+      <c r="A129" s="47"/>
       <c r="B129" s="13">
         <v>5</v>
       </c>
@@ -20960,7 +20960,7 @@
       </c>
     </row>
     <row r="130" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A130" s="48"/>
+      <c r="A130" s="47"/>
       <c r="B130" s="13">
         <v>6</v>
       </c>
@@ -21090,7 +21090,7 @@
       </c>
     </row>
     <row r="131" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A131" s="48"/>
+      <c r="A131" s="47"/>
       <c r="B131" s="13">
         <v>7</v>
       </c>
@@ -21220,7 +21220,7 @@
       </c>
     </row>
     <row r="132" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A132" s="48"/>
+      <c r="A132" s="47"/>
       <c r="B132" s="13">
         <v>8</v>
       </c>
@@ -21350,7 +21350,7 @@
       </c>
     </row>
     <row r="133" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A133" s="48"/>
+      <c r="A133" s="47"/>
       <c r="B133" s="13">
         <v>9</v>
       </c>
@@ -21480,7 +21480,7 @@
       </c>
     </row>
     <row r="134" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A134" s="48"/>
+      <c r="A134" s="47"/>
       <c r="B134" s="13">
         <v>10</v>
       </c>
@@ -21610,7 +21610,7 @@
       </c>
     </row>
     <row r="135" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A135" s="48"/>
+      <c r="A135" s="47"/>
       <c r="B135" s="13">
         <v>11</v>
       </c>
@@ -21740,7 +21740,7 @@
       </c>
     </row>
     <row r="136" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A136" s="48"/>
+      <c r="A136" s="47"/>
       <c r="B136" s="13">
         <v>12</v>
       </c>
@@ -21870,7 +21870,7 @@
       </c>
     </row>
     <row r="137" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A137" s="48"/>
+      <c r="A137" s="47"/>
       <c r="B137" s="13">
         <v>13</v>
       </c>
@@ -22000,7 +22000,7 @@
       </c>
     </row>
     <row r="138" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A138" s="48"/>
+      <c r="A138" s="47"/>
       <c r="B138" s="13">
         <v>14</v>
       </c>
@@ -22130,7 +22130,7 @@
       </c>
     </row>
     <row r="139" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A139" s="48"/>
+      <c r="A139" s="47"/>
       <c r="B139" s="13">
         <v>15</v>
       </c>
@@ -22260,7 +22260,7 @@
       </c>
     </row>
     <row r="140" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A140" s="48"/>
+      <c r="A140" s="47"/>
       <c r="B140" s="13">
         <v>16</v>
       </c>
@@ -22390,7 +22390,7 @@
       </c>
     </row>
     <row r="141" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A141" s="48"/>
+      <c r="A141" s="47"/>
       <c r="B141" s="13">
         <v>17</v>
       </c>
@@ -22520,7 +22520,7 @@
       </c>
     </row>
     <row r="142" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A142" s="48"/>
+      <c r="A142" s="47"/>
       <c r="B142" s="13">
         <v>18</v>
       </c>
@@ -22650,7 +22650,7 @@
       </c>
     </row>
     <row r="143" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A143" s="48"/>
+      <c r="A143" s="47"/>
       <c r="B143" s="13">
         <v>19</v>
       </c>
@@ -22780,7 +22780,7 @@
       </c>
     </row>
     <row r="144" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A144" s="48"/>
+      <c r="A144" s="47"/>
       <c r="B144" s="13">
         <v>20</v>
       </c>
@@ -22910,7 +22910,7 @@
       </c>
     </row>
     <row r="145" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A145" s="48"/>
+      <c r="A145" s="47"/>
       <c r="B145" s="13">
         <v>21</v>
       </c>
@@ -23040,7 +23040,7 @@
       </c>
     </row>
     <row r="146" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A146" s="48"/>
+      <c r="A146" s="47"/>
       <c r="B146" s="13">
         <v>22</v>
       </c>
@@ -23170,7 +23170,7 @@
       </c>
     </row>
     <row r="147" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A147" s="48"/>
+      <c r="A147" s="47"/>
       <c r="B147" s="13">
         <v>23</v>
       </c>
@@ -23300,7 +23300,7 @@
       </c>
     </row>
     <row r="148" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A148" s="48"/>
+      <c r="A148" s="47"/>
       <c r="B148" s="13">
         <v>24</v>
       </c>
@@ -23430,7 +23430,7 @@
       </c>
     </row>
     <row r="149" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A149" s="48"/>
+      <c r="A149" s="47"/>
       <c r="B149" s="13">
         <v>25</v>
       </c>
@@ -23560,7 +23560,7 @@
       </c>
     </row>
     <row r="150" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A150" s="48"/>
+      <c r="A150" s="47"/>
       <c r="B150" s="13">
         <v>26</v>
       </c>
@@ -23690,7 +23690,7 @@
       </c>
     </row>
     <row r="151" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A151" s="48"/>
+      <c r="A151" s="47"/>
       <c r="B151" s="13">
         <v>27</v>
       </c>
@@ -23820,7 +23820,7 @@
       </c>
     </row>
     <row r="152" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A152" s="48"/>
+      <c r="A152" s="47"/>
       <c r="B152" s="13">
         <v>28</v>
       </c>
@@ -23950,7 +23950,7 @@
       </c>
     </row>
     <row r="153" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A153" s="48"/>
+      <c r="A153" s="47"/>
       <c r="B153" s="13">
         <v>29</v>
       </c>
@@ -24080,7 +24080,7 @@
       </c>
     </row>
     <row r="154" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A154" s="48"/>
+      <c r="A154" s="47"/>
       <c r="B154" s="13">
         <v>30</v>
       </c>
@@ -24210,7 +24210,7 @@
       </c>
     </row>
     <row r="155" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A155" s="48"/>
+      <c r="A155" s="47"/>
       <c r="B155" s="13">
         <v>31</v>
       </c>
@@ -24340,7 +24340,7 @@
       </c>
     </row>
     <row r="156" spans="1:373" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A156" s="48"/>
+      <c r="A156" s="47"/>
       <c r="B156" s="16">
         <v>32</v>
       </c>
@@ -24799,7 +24799,7 @@
       <c r="NI156" s="2"/>
     </row>
     <row r="157" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A157" s="48"/>
+      <c r="A157" s="47"/>
       <c r="B157" s="13">
         <v>33</v>
       </c>
@@ -24928,7 +24928,7 @@
       </c>
     </row>
     <row r="158" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A158" s="48"/>
+      <c r="A158" s="47"/>
       <c r="B158" s="13">
         <v>34</v>
       </c>
@@ -24936,7 +24936,7 @@
         <v>54</v>
       </c>
       <c r="D158" s="37">
-        <v>0.45</v>
+        <v>0.6</v>
       </c>
       <c r="E158" s="4">
         <v>0</v>
@@ -25057,7 +25057,7 @@
       </c>
     </row>
     <row r="159" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A159" s="48"/>
+      <c r="A159" s="47"/>
       <c r="B159" s="13">
         <v>35</v>
       </c>
@@ -25186,7 +25186,7 @@
       </c>
     </row>
     <row r="160" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A160" s="48"/>
+      <c r="A160" s="47"/>
       <c r="B160" s="13">
         <v>36</v>
       </c>
@@ -25315,7 +25315,7 @@
       </c>
     </row>
     <row r="161" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A161" s="48"/>
+      <c r="A161" s="47"/>
       <c r="B161" s="13">
         <v>37</v>
       </c>
@@ -25444,7 +25444,7 @@
       </c>
     </row>
     <row r="162" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A162" s="48"/>
+      <c r="A162" s="47"/>
       <c r="B162" s="13">
         <v>38</v>
       </c>
@@ -25573,7 +25573,7 @@
       </c>
     </row>
     <row r="163" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A163" s="48"/>
+      <c r="A163" s="47"/>
       <c r="B163" s="13">
         <v>39</v>
       </c>
@@ -25702,7 +25702,7 @@
       </c>
     </row>
     <row r="164" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A164" s="49"/>
+      <c r="A164" s="48"/>
       <c r="B164" s="20">
         <v>40</v>
       </c>
@@ -25831,7 +25831,7 @@
       </c>
     </row>
     <row r="165" spans="1:373" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A165" s="46">
+      <c r="A165" s="49">
         <v>5</v>
       </c>
       <c r="B165" s="13">
@@ -26293,7 +26293,7 @@
       <c r="NI165"/>
     </row>
     <row r="166" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A166" s="46"/>
+      <c r="A166" s="49"/>
       <c r="B166" s="13">
         <v>2</v>
       </c>
@@ -26423,7 +26423,7 @@
       </c>
     </row>
     <row r="167" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A167" s="46"/>
+      <c r="A167" s="49"/>
       <c r="B167" s="13">
         <v>3</v>
       </c>
@@ -26553,7 +26553,7 @@
       </c>
     </row>
     <row r="168" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A168" s="46"/>
+      <c r="A168" s="49"/>
       <c r="B168" s="13">
         <v>4</v>
       </c>
@@ -26683,7 +26683,7 @@
       </c>
     </row>
     <row r="169" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A169" s="46"/>
+      <c r="A169" s="49"/>
       <c r="B169" s="13">
         <v>5</v>
       </c>
@@ -26813,7 +26813,7 @@
       </c>
     </row>
     <row r="170" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A170" s="46"/>
+      <c r="A170" s="49"/>
       <c r="B170" s="13">
         <v>6</v>
       </c>
@@ -26943,7 +26943,7 @@
       </c>
     </row>
     <row r="171" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A171" s="46"/>
+      <c r="A171" s="49"/>
       <c r="B171" s="13">
         <v>7</v>
       </c>
@@ -27073,7 +27073,7 @@
       </c>
     </row>
     <row r="172" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A172" s="46"/>
+      <c r="A172" s="49"/>
       <c r="B172" s="13">
         <v>8</v>
       </c>
@@ -27203,7 +27203,7 @@
       </c>
     </row>
     <row r="173" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A173" s="46"/>
+      <c r="A173" s="49"/>
       <c r="B173" s="13">
         <v>9</v>
       </c>
@@ -27333,7 +27333,7 @@
       </c>
     </row>
     <row r="174" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A174" s="46"/>
+      <c r="A174" s="49"/>
       <c r="B174" s="13">
         <v>10</v>
       </c>
@@ -27463,7 +27463,7 @@
       </c>
     </row>
     <row r="175" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A175" s="46"/>
+      <c r="A175" s="49"/>
       <c r="B175" s="13">
         <v>11</v>
       </c>
@@ -27593,7 +27593,7 @@
       </c>
     </row>
     <row r="176" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A176" s="46"/>
+      <c r="A176" s="49"/>
       <c r="B176" s="13">
         <v>12</v>
       </c>
@@ -27723,7 +27723,7 @@
       </c>
     </row>
     <row r="177" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A177" s="46"/>
+      <c r="A177" s="49"/>
       <c r="B177" s="13">
         <v>13</v>
       </c>
@@ -27853,7 +27853,7 @@
       </c>
     </row>
     <row r="178" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A178" s="46"/>
+      <c r="A178" s="49"/>
       <c r="B178" s="13">
         <v>14</v>
       </c>
@@ -27983,7 +27983,7 @@
       </c>
     </row>
     <row r="179" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A179" s="46"/>
+      <c r="A179" s="49"/>
       <c r="B179" s="13">
         <v>15</v>
       </c>
@@ -28113,7 +28113,7 @@
       </c>
     </row>
     <row r="180" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A180" s="46"/>
+      <c r="A180" s="49"/>
       <c r="B180" s="13">
         <v>16</v>
       </c>
@@ -28243,7 +28243,7 @@
       </c>
     </row>
     <row r="181" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A181" s="46"/>
+      <c r="A181" s="49"/>
       <c r="B181" s="13">
         <v>17</v>
       </c>
@@ -28373,7 +28373,7 @@
       </c>
     </row>
     <row r="182" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A182" s="46"/>
+      <c r="A182" s="49"/>
       <c r="B182" s="13">
         <v>18</v>
       </c>
@@ -28503,7 +28503,7 @@
       </c>
     </row>
     <row r="183" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A183" s="46"/>
+      <c r="A183" s="49"/>
       <c r="B183" s="13">
         <v>19</v>
       </c>
@@ -28633,7 +28633,7 @@
       </c>
     </row>
     <row r="184" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A184" s="46"/>
+      <c r="A184" s="49"/>
       <c r="B184" s="13">
         <v>20</v>
       </c>
@@ -28763,7 +28763,7 @@
       </c>
     </row>
     <row r="185" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A185" s="46"/>
+      <c r="A185" s="49"/>
       <c r="B185" s="13">
         <v>21</v>
       </c>
@@ -28893,7 +28893,7 @@
       </c>
     </row>
     <row r="186" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A186" s="46"/>
+      <c r="A186" s="49"/>
       <c r="B186" s="13">
         <v>22</v>
       </c>
@@ -29023,7 +29023,7 @@
       </c>
     </row>
     <row r="187" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A187" s="46"/>
+      <c r="A187" s="49"/>
       <c r="B187" s="13">
         <v>23</v>
       </c>
@@ -29153,7 +29153,7 @@
       </c>
     </row>
     <row r="188" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A188" s="46"/>
+      <c r="A188" s="49"/>
       <c r="B188" s="13">
         <v>24</v>
       </c>
@@ -29283,7 +29283,7 @@
       </c>
     </row>
     <row r="189" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A189" s="46"/>
+      <c r="A189" s="49"/>
       <c r="B189" s="13">
         <v>25</v>
       </c>
@@ -29413,7 +29413,7 @@
       </c>
     </row>
     <row r="190" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A190" s="46"/>
+      <c r="A190" s="49"/>
       <c r="B190" s="13">
         <v>26</v>
       </c>
@@ -29543,7 +29543,7 @@
       </c>
     </row>
     <row r="191" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A191" s="46"/>
+      <c r="A191" s="49"/>
       <c r="B191" s="13">
         <v>27</v>
       </c>
@@ -29673,7 +29673,7 @@
       </c>
     </row>
     <row r="192" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A192" s="46"/>
+      <c r="A192" s="49"/>
       <c r="B192" s="13">
         <v>28</v>
       </c>
@@ -29803,7 +29803,7 @@
       </c>
     </row>
     <row r="193" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A193" s="46"/>
+      <c r="A193" s="49"/>
       <c r="B193" s="13">
         <v>29</v>
       </c>
@@ -29933,7 +29933,7 @@
       </c>
     </row>
     <row r="194" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A194" s="46"/>
+      <c r="A194" s="49"/>
       <c r="B194" s="13">
         <v>30</v>
       </c>
@@ -30063,7 +30063,7 @@
       </c>
     </row>
     <row r="195" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A195" s="46"/>
+      <c r="A195" s="49"/>
       <c r="B195" s="13">
         <v>31</v>
       </c>
@@ -30193,7 +30193,7 @@
       </c>
     </row>
     <row r="196" spans="1:373" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A196" s="46"/>
+      <c r="A196" s="49"/>
       <c r="B196" s="16">
         <v>32</v>
       </c>
@@ -30652,7 +30652,7 @@
       <c r="NI196" s="2"/>
     </row>
     <row r="197" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A197" s="46"/>
+      <c r="A197" s="49"/>
       <c r="B197" s="13">
         <v>33</v>
       </c>
@@ -30781,7 +30781,7 @@
       </c>
     </row>
     <row r="198" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A198" s="46"/>
+      <c r="A198" s="49"/>
       <c r="B198" s="13">
         <v>34</v>
       </c>
@@ -30789,7 +30789,7 @@
         <v>54</v>
       </c>
       <c r="D198" s="37">
-        <v>0.45</v>
+        <v>0.6</v>
       </c>
       <c r="E198" s="4">
         <v>0</v>
@@ -30910,7 +30910,7 @@
       </c>
     </row>
     <row r="199" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A199" s="46"/>
+      <c r="A199" s="49"/>
       <c r="B199" s="13">
         <v>35</v>
       </c>
@@ -31039,7 +31039,7 @@
       </c>
     </row>
     <row r="200" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A200" s="46"/>
+      <c r="A200" s="49"/>
       <c r="B200" s="13">
         <v>36</v>
       </c>
@@ -31168,7 +31168,7 @@
       </c>
     </row>
     <row r="201" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A201" s="46"/>
+      <c r="A201" s="49"/>
       <c r="B201" s="13">
         <v>37</v>
       </c>
@@ -31297,7 +31297,7 @@
       </c>
     </row>
     <row r="202" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A202" s="46"/>
+      <c r="A202" s="49"/>
       <c r="B202" s="13">
         <v>38</v>
       </c>
@@ -31426,7 +31426,7 @@
       </c>
     </row>
     <row r="203" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A203" s="46"/>
+      <c r="A203" s="49"/>
       <c r="B203" s="13">
         <v>39</v>
       </c>
@@ -31555,7 +31555,7 @@
       </c>
     </row>
     <row r="204" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A204" s="46"/>
+      <c r="A204" s="49"/>
       <c r="B204" s="13">
         <v>40</v>
       </c>
@@ -31684,7 +31684,7 @@
       </c>
     </row>
     <row r="205" spans="1:373" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A205" s="47">
+      <c r="A205" s="46">
         <v>6</v>
       </c>
       <c r="B205" s="16">
@@ -32146,7 +32146,7 @@
       <c r="NI205"/>
     </row>
     <row r="206" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A206" s="48"/>
+      <c r="A206" s="47"/>
       <c r="B206" s="13">
         <v>2</v>
       </c>
@@ -32276,7 +32276,7 @@
       </c>
     </row>
     <row r="207" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A207" s="48"/>
+      <c r="A207" s="47"/>
       <c r="B207" s="13">
         <v>3</v>
       </c>
@@ -32406,7 +32406,7 @@
       </c>
     </row>
     <row r="208" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A208" s="48"/>
+      <c r="A208" s="47"/>
       <c r="B208" s="13">
         <v>4</v>
       </c>
@@ -32536,7 +32536,7 @@
       </c>
     </row>
     <row r="209" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A209" s="48"/>
+      <c r="A209" s="47"/>
       <c r="B209" s="13">
         <v>5</v>
       </c>
@@ -32666,7 +32666,7 @@
       </c>
     </row>
     <row r="210" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A210" s="48"/>
+      <c r="A210" s="47"/>
       <c r="B210" s="13">
         <v>6</v>
       </c>
@@ -32796,7 +32796,7 @@
       </c>
     </row>
     <row r="211" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A211" s="48"/>
+      <c r="A211" s="47"/>
       <c r="B211" s="13">
         <v>7</v>
       </c>
@@ -32926,7 +32926,7 @@
       </c>
     </row>
     <row r="212" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A212" s="48"/>
+      <c r="A212" s="47"/>
       <c r="B212" s="13">
         <v>8</v>
       </c>
@@ -33056,7 +33056,7 @@
       </c>
     </row>
     <row r="213" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A213" s="48"/>
+      <c r="A213" s="47"/>
       <c r="B213" s="13">
         <v>9</v>
       </c>
@@ -33186,7 +33186,7 @@
       </c>
     </row>
     <row r="214" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A214" s="48"/>
+      <c r="A214" s="47"/>
       <c r="B214" s="13">
         <v>10</v>
       </c>
@@ -33316,7 +33316,7 @@
       </c>
     </row>
     <row r="215" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A215" s="48"/>
+      <c r="A215" s="47"/>
       <c r="B215" s="13">
         <v>11</v>
       </c>
@@ -33446,7 +33446,7 @@
       </c>
     </row>
     <row r="216" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A216" s="48"/>
+      <c r="A216" s="47"/>
       <c r="B216" s="13">
         <v>12</v>
       </c>
@@ -33576,7 +33576,7 @@
       </c>
     </row>
     <row r="217" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A217" s="48"/>
+      <c r="A217" s="47"/>
       <c r="B217" s="13">
         <v>13</v>
       </c>
@@ -33706,7 +33706,7 @@
       </c>
     </row>
     <row r="218" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A218" s="48"/>
+      <c r="A218" s="47"/>
       <c r="B218" s="13">
         <v>14</v>
       </c>
@@ -33836,7 +33836,7 @@
       </c>
     </row>
     <row r="219" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A219" s="48"/>
+      <c r="A219" s="47"/>
       <c r="B219" s="13">
         <v>15</v>
       </c>
@@ -33966,7 +33966,7 @@
       </c>
     </row>
     <row r="220" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A220" s="48"/>
+      <c r="A220" s="47"/>
       <c r="B220" s="13">
         <v>16</v>
       </c>
@@ -34096,7 +34096,7 @@
       </c>
     </row>
     <row r="221" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A221" s="48"/>
+      <c r="A221" s="47"/>
       <c r="B221" s="13">
         <v>17</v>
       </c>
@@ -34226,7 +34226,7 @@
       </c>
     </row>
     <row r="222" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A222" s="48"/>
+      <c r="A222" s="47"/>
       <c r="B222" s="13">
         <v>18</v>
       </c>
@@ -34356,7 +34356,7 @@
       </c>
     </row>
     <row r="223" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A223" s="48"/>
+      <c r="A223" s="47"/>
       <c r="B223" s="13">
         <v>19</v>
       </c>
@@ -34486,7 +34486,7 @@
       </c>
     </row>
     <row r="224" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A224" s="48"/>
+      <c r="A224" s="47"/>
       <c r="B224" s="13">
         <v>20</v>
       </c>
@@ -34616,7 +34616,7 @@
       </c>
     </row>
     <row r="225" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A225" s="48"/>
+      <c r="A225" s="47"/>
       <c r="B225" s="13">
         <v>21</v>
       </c>
@@ -34746,7 +34746,7 @@
       </c>
     </row>
     <row r="226" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A226" s="48"/>
+      <c r="A226" s="47"/>
       <c r="B226" s="13">
         <v>22</v>
       </c>
@@ -34876,7 +34876,7 @@
       </c>
     </row>
     <row r="227" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A227" s="48"/>
+      <c r="A227" s="47"/>
       <c r="B227" s="13">
         <v>23</v>
       </c>
@@ -35006,7 +35006,7 @@
       </c>
     </row>
     <row r="228" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A228" s="48"/>
+      <c r="A228" s="47"/>
       <c r="B228" s="13">
         <v>24</v>
       </c>
@@ -35136,7 +35136,7 @@
       </c>
     </row>
     <row r="229" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A229" s="48"/>
+      <c r="A229" s="47"/>
       <c r="B229" s="13">
         <v>25</v>
       </c>
@@ -35266,7 +35266,7 @@
       </c>
     </row>
     <row r="230" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A230" s="48"/>
+      <c r="A230" s="47"/>
       <c r="B230" s="13">
         <v>26</v>
       </c>
@@ -35396,7 +35396,7 @@
       </c>
     </row>
     <row r="231" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A231" s="48"/>
+      <c r="A231" s="47"/>
       <c r="B231" s="13">
         <v>27</v>
       </c>
@@ -35526,7 +35526,7 @@
       </c>
     </row>
     <row r="232" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A232" s="48"/>
+      <c r="A232" s="47"/>
       <c r="B232" s="13">
         <v>28</v>
       </c>
@@ -35656,7 +35656,7 @@
       </c>
     </row>
     <row r="233" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A233" s="48"/>
+      <c r="A233" s="47"/>
       <c r="B233" s="13">
         <v>29</v>
       </c>
@@ -35786,7 +35786,7 @@
       </c>
     </row>
     <row r="234" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A234" s="48"/>
+      <c r="A234" s="47"/>
       <c r="B234" s="13">
         <v>30</v>
       </c>
@@ -35916,7 +35916,7 @@
       </c>
     </row>
     <row r="235" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A235" s="48"/>
+      <c r="A235" s="47"/>
       <c r="B235" s="13">
         <v>31</v>
       </c>
@@ -36046,7 +36046,7 @@
       </c>
     </row>
     <row r="236" spans="1:373" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A236" s="48"/>
+      <c r="A236" s="47"/>
       <c r="B236" s="16">
         <v>32</v>
       </c>
@@ -36505,7 +36505,7 @@
       <c r="NI236" s="2"/>
     </row>
     <row r="237" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A237" s="48"/>
+      <c r="A237" s="47"/>
       <c r="B237" s="13">
         <v>33</v>
       </c>
@@ -36634,7 +36634,7 @@
       </c>
     </row>
     <row r="238" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A238" s="48"/>
+      <c r="A238" s="47"/>
       <c r="B238" s="13">
         <v>34</v>
       </c>
@@ -36642,7 +36642,7 @@
         <v>54</v>
       </c>
       <c r="D238" s="37">
-        <v>0.45</v>
+        <v>0.6</v>
       </c>
       <c r="E238" s="4">
         <v>0</v>
@@ -36763,7 +36763,7 @@
       </c>
     </row>
     <row r="239" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A239" s="48"/>
+      <c r="A239" s="47"/>
       <c r="B239" s="13">
         <v>35</v>
       </c>
@@ -36892,7 +36892,7 @@
       </c>
     </row>
     <row r="240" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A240" s="48"/>
+      <c r="A240" s="47"/>
       <c r="B240" s="13">
         <v>36</v>
       </c>
@@ -37021,7 +37021,7 @@
       </c>
     </row>
     <row r="241" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A241" s="48"/>
+      <c r="A241" s="47"/>
       <c r="B241" s="13">
         <v>37</v>
       </c>
@@ -37150,7 +37150,7 @@
       </c>
     </row>
     <row r="242" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A242" s="48"/>
+      <c r="A242" s="47"/>
       <c r="B242" s="13">
         <v>38</v>
       </c>
@@ -37279,7 +37279,7 @@
       </c>
     </row>
     <row r="243" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A243" s="48"/>
+      <c r="A243" s="47"/>
       <c r="B243" s="13">
         <v>39</v>
       </c>
@@ -37408,7 +37408,7 @@
       </c>
     </row>
     <row r="244" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A244" s="49"/>
+      <c r="A244" s="48"/>
       <c r="B244" s="20">
         <v>40</v>
       </c>
@@ -37537,7 +37537,7 @@
       </c>
     </row>
     <row r="245" spans="1:373" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A245" s="46">
+      <c r="A245" s="49">
         <v>7</v>
       </c>
       <c r="B245" s="13">
@@ -37999,7 +37999,7 @@
       <c r="NI245"/>
     </row>
     <row r="246" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A246" s="46"/>
+      <c r="A246" s="49"/>
       <c r="B246" s="13">
         <v>2</v>
       </c>
@@ -38129,7 +38129,7 @@
       </c>
     </row>
     <row r="247" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A247" s="46"/>
+      <c r="A247" s="49"/>
       <c r="B247" s="13">
         <v>3</v>
       </c>
@@ -38259,7 +38259,7 @@
       </c>
     </row>
     <row r="248" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A248" s="46"/>
+      <c r="A248" s="49"/>
       <c r="B248" s="13">
         <v>4</v>
       </c>
@@ -38389,7 +38389,7 @@
       </c>
     </row>
     <row r="249" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A249" s="46"/>
+      <c r="A249" s="49"/>
       <c r="B249" s="13">
         <v>5</v>
       </c>
@@ -38519,7 +38519,7 @@
       </c>
     </row>
     <row r="250" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A250" s="46"/>
+      <c r="A250" s="49"/>
       <c r="B250" s="13">
         <v>6</v>
       </c>
@@ -38649,7 +38649,7 @@
       </c>
     </row>
     <row r="251" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A251" s="46"/>
+      <c r="A251" s="49"/>
       <c r="B251" s="13">
         <v>7</v>
       </c>
@@ -38779,7 +38779,7 @@
       </c>
     </row>
     <row r="252" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A252" s="46"/>
+      <c r="A252" s="49"/>
       <c r="B252" s="13">
         <v>8</v>
       </c>
@@ -38909,7 +38909,7 @@
       </c>
     </row>
     <row r="253" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A253" s="46"/>
+      <c r="A253" s="49"/>
       <c r="B253" s="13">
         <v>9</v>
       </c>
@@ -39039,7 +39039,7 @@
       </c>
     </row>
     <row r="254" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A254" s="46"/>
+      <c r="A254" s="49"/>
       <c r="B254" s="13">
         <v>10</v>
       </c>
@@ -39169,7 +39169,7 @@
       </c>
     </row>
     <row r="255" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A255" s="46"/>
+      <c r="A255" s="49"/>
       <c r="B255" s="13">
         <v>11</v>
       </c>
@@ -39299,7 +39299,7 @@
       </c>
     </row>
     <row r="256" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A256" s="46"/>
+      <c r="A256" s="49"/>
       <c r="B256" s="13">
         <v>12</v>
       </c>
@@ -39429,7 +39429,7 @@
       </c>
     </row>
     <row r="257" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A257" s="46"/>
+      <c r="A257" s="49"/>
       <c r="B257" s="13">
         <v>13</v>
       </c>
@@ -39559,7 +39559,7 @@
       </c>
     </row>
     <row r="258" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A258" s="46"/>
+      <c r="A258" s="49"/>
       <c r="B258" s="13">
         <v>14</v>
       </c>
@@ -39689,7 +39689,7 @@
       </c>
     </row>
     <row r="259" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A259" s="46"/>
+      <c r="A259" s="49"/>
       <c r="B259" s="13">
         <v>15</v>
       </c>
@@ -39819,7 +39819,7 @@
       </c>
     </row>
     <row r="260" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A260" s="46"/>
+      <c r="A260" s="49"/>
       <c r="B260" s="13">
         <v>16</v>
       </c>
@@ -39949,7 +39949,7 @@
       </c>
     </row>
     <row r="261" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A261" s="46"/>
+      <c r="A261" s="49"/>
       <c r="B261" s="13">
         <v>17</v>
       </c>
@@ -40079,7 +40079,7 @@
       </c>
     </row>
     <row r="262" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A262" s="46"/>
+      <c r="A262" s="49"/>
       <c r="B262" s="13">
         <v>18</v>
       </c>
@@ -40209,7 +40209,7 @@
       </c>
     </row>
     <row r="263" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A263" s="46"/>
+      <c r="A263" s="49"/>
       <c r="B263" s="13">
         <v>19</v>
       </c>
@@ -40339,7 +40339,7 @@
       </c>
     </row>
     <row r="264" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A264" s="46"/>
+      <c r="A264" s="49"/>
       <c r="B264" s="13">
         <v>20</v>
       </c>
@@ -40469,7 +40469,7 @@
       </c>
     </row>
     <row r="265" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A265" s="46"/>
+      <c r="A265" s="49"/>
       <c r="B265" s="13">
         <v>21</v>
       </c>
@@ -40599,7 +40599,7 @@
       </c>
     </row>
     <row r="266" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A266" s="46"/>
+      <c r="A266" s="49"/>
       <c r="B266" s="13">
         <v>22</v>
       </c>
@@ -40729,7 +40729,7 @@
       </c>
     </row>
     <row r="267" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A267" s="46"/>
+      <c r="A267" s="49"/>
       <c r="B267" s="13">
         <v>23</v>
       </c>
@@ -40859,7 +40859,7 @@
       </c>
     </row>
     <row r="268" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A268" s="46"/>
+      <c r="A268" s="49"/>
       <c r="B268" s="13">
         <v>24</v>
       </c>
@@ -40989,7 +40989,7 @@
       </c>
     </row>
     <row r="269" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A269" s="46"/>
+      <c r="A269" s="49"/>
       <c r="B269" s="13">
         <v>25</v>
       </c>
@@ -41119,7 +41119,7 @@
       </c>
     </row>
     <row r="270" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A270" s="46"/>
+      <c r="A270" s="49"/>
       <c r="B270" s="13">
         <v>26</v>
       </c>
@@ -41249,7 +41249,7 @@
       </c>
     </row>
     <row r="271" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A271" s="46"/>
+      <c r="A271" s="49"/>
       <c r="B271" s="13">
         <v>27</v>
       </c>
@@ -41379,7 +41379,7 @@
       </c>
     </row>
     <row r="272" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A272" s="46"/>
+      <c r="A272" s="49"/>
       <c r="B272" s="13">
         <v>28</v>
       </c>
@@ -41509,7 +41509,7 @@
       </c>
     </row>
     <row r="273" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A273" s="46"/>
+      <c r="A273" s="49"/>
       <c r="B273" s="13">
         <v>29</v>
       </c>
@@ -41639,7 +41639,7 @@
       </c>
     </row>
     <row r="274" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A274" s="46"/>
+      <c r="A274" s="49"/>
       <c r="B274" s="13">
         <v>30</v>
       </c>
@@ -41769,7 +41769,7 @@
       </c>
     </row>
     <row r="275" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A275" s="46"/>
+      <c r="A275" s="49"/>
       <c r="B275" s="13">
         <v>31</v>
       </c>
@@ -41899,7 +41899,7 @@
       </c>
     </row>
     <row r="276" spans="1:373" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A276" s="46"/>
+      <c r="A276" s="49"/>
       <c r="B276" s="16">
         <v>32</v>
       </c>
@@ -42358,7 +42358,7 @@
       <c r="NI276" s="2"/>
     </row>
     <row r="277" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A277" s="46"/>
+      <c r="A277" s="49"/>
       <c r="B277" s="13">
         <v>33</v>
       </c>
@@ -42487,7 +42487,7 @@
       </c>
     </row>
     <row r="278" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A278" s="46"/>
+      <c r="A278" s="49"/>
       <c r="B278" s="13">
         <v>34</v>
       </c>
@@ -42495,7 +42495,7 @@
         <v>54</v>
       </c>
       <c r="D278" s="3">
-        <v>0.55000000000000004</v>
+        <v>0.7</v>
       </c>
       <c r="E278" s="4">
         <v>0</v>
@@ -42616,7 +42616,7 @@
       </c>
     </row>
     <row r="279" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A279" s="46"/>
+      <c r="A279" s="49"/>
       <c r="B279" s="13">
         <v>35</v>
       </c>
@@ -42745,7 +42745,7 @@
       </c>
     </row>
     <row r="280" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A280" s="46"/>
+      <c r="A280" s="49"/>
       <c r="B280" s="13">
         <v>36</v>
       </c>
@@ -42874,7 +42874,7 @@
       </c>
     </row>
     <row r="281" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A281" s="46"/>
+      <c r="A281" s="49"/>
       <c r="B281" s="13">
         <v>37</v>
       </c>
@@ -43003,7 +43003,7 @@
       </c>
     </row>
     <row r="282" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A282" s="46"/>
+      <c r="A282" s="49"/>
       <c r="B282" s="13">
         <v>38</v>
       </c>
@@ -43132,7 +43132,7 @@
       </c>
     </row>
     <row r="283" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A283" s="46"/>
+      <c r="A283" s="49"/>
       <c r="B283" s="13">
         <v>39</v>
       </c>
@@ -43261,7 +43261,7 @@
       </c>
     </row>
     <row r="284" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A284" s="46"/>
+      <c r="A284" s="49"/>
       <c r="B284" s="13">
         <v>40</v>
       </c>
@@ -43390,7 +43390,7 @@
       </c>
     </row>
     <row r="285" spans="1:373" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A285" s="47">
+      <c r="A285" s="46">
         <v>8</v>
       </c>
       <c r="B285" s="16">
@@ -43852,7 +43852,7 @@
       <c r="NI285"/>
     </row>
     <row r="286" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A286" s="48"/>
+      <c r="A286" s="47"/>
       <c r="B286" s="13">
         <v>2</v>
       </c>
@@ -43982,7 +43982,7 @@
       </c>
     </row>
     <row r="287" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A287" s="48"/>
+      <c r="A287" s="47"/>
       <c r="B287" s="13">
         <v>3</v>
       </c>
@@ -44112,7 +44112,7 @@
       </c>
     </row>
     <row r="288" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A288" s="48"/>
+      <c r="A288" s="47"/>
       <c r="B288" s="13">
         <v>4</v>
       </c>
@@ -44242,7 +44242,7 @@
       </c>
     </row>
     <row r="289" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A289" s="48"/>
+      <c r="A289" s="47"/>
       <c r="B289" s="13">
         <v>5</v>
       </c>
@@ -44372,7 +44372,7 @@
       </c>
     </row>
     <row r="290" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A290" s="48"/>
+      <c r="A290" s="47"/>
       <c r="B290" s="13">
         <v>6</v>
       </c>
@@ -44502,7 +44502,7 @@
       </c>
     </row>
     <row r="291" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A291" s="48"/>
+      <c r="A291" s="47"/>
       <c r="B291" s="13">
         <v>7</v>
       </c>
@@ -44632,7 +44632,7 @@
       </c>
     </row>
     <row r="292" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A292" s="48"/>
+      <c r="A292" s="47"/>
       <c r="B292" s="13">
         <v>8</v>
       </c>
@@ -44762,7 +44762,7 @@
       </c>
     </row>
     <row r="293" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A293" s="48"/>
+      <c r="A293" s="47"/>
       <c r="B293" s="13">
         <v>9</v>
       </c>
@@ -44892,7 +44892,7 @@
       </c>
     </row>
     <row r="294" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A294" s="48"/>
+      <c r="A294" s="47"/>
       <c r="B294" s="13">
         <v>10</v>
       </c>
@@ -45022,7 +45022,7 @@
       </c>
     </row>
     <row r="295" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A295" s="48"/>
+      <c r="A295" s="47"/>
       <c r="B295" s="13">
         <v>11</v>
       </c>
@@ -45152,7 +45152,7 @@
       </c>
     </row>
     <row r="296" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A296" s="48"/>
+      <c r="A296" s="47"/>
       <c r="B296" s="13">
         <v>12</v>
       </c>
@@ -45282,7 +45282,7 @@
       </c>
     </row>
     <row r="297" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A297" s="48"/>
+      <c r="A297" s="47"/>
       <c r="B297" s="13">
         <v>13</v>
       </c>
@@ -45412,7 +45412,7 @@
       </c>
     </row>
     <row r="298" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A298" s="48"/>
+      <c r="A298" s="47"/>
       <c r="B298" s="13">
         <v>14</v>
       </c>
@@ -45542,7 +45542,7 @@
       </c>
     </row>
     <row r="299" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A299" s="48"/>
+      <c r="A299" s="47"/>
       <c r="B299" s="13">
         <v>15</v>
       </c>
@@ -45672,7 +45672,7 @@
       </c>
     </row>
     <row r="300" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A300" s="48"/>
+      <c r="A300" s="47"/>
       <c r="B300" s="13">
         <v>16</v>
       </c>
@@ -45802,7 +45802,7 @@
       </c>
     </row>
     <row r="301" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A301" s="48"/>
+      <c r="A301" s="47"/>
       <c r="B301" s="13">
         <v>17</v>
       </c>
@@ -45932,7 +45932,7 @@
       </c>
     </row>
     <row r="302" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A302" s="48"/>
+      <c r="A302" s="47"/>
       <c r="B302" s="13">
         <v>18</v>
       </c>
@@ -46062,7 +46062,7 @@
       </c>
     </row>
     <row r="303" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A303" s="48"/>
+      <c r="A303" s="47"/>
       <c r="B303" s="13">
         <v>19</v>
       </c>
@@ -46192,7 +46192,7 @@
       </c>
     </row>
     <row r="304" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A304" s="48"/>
+      <c r="A304" s="47"/>
       <c r="B304" s="13">
         <v>20</v>
       </c>
@@ -46322,7 +46322,7 @@
       </c>
     </row>
     <row r="305" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A305" s="48"/>
+      <c r="A305" s="47"/>
       <c r="B305" s="13">
         <v>21</v>
       </c>
@@ -46452,7 +46452,7 @@
       </c>
     </row>
     <row r="306" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A306" s="48"/>
+      <c r="A306" s="47"/>
       <c r="B306" s="13">
         <v>22</v>
       </c>
@@ -46582,7 +46582,7 @@
       </c>
     </row>
     <row r="307" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A307" s="48"/>
+      <c r="A307" s="47"/>
       <c r="B307" s="13">
         <v>23</v>
       </c>
@@ -46712,7 +46712,7 @@
       </c>
     </row>
     <row r="308" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A308" s="48"/>
+      <c r="A308" s="47"/>
       <c r="B308" s="13">
         <v>24</v>
       </c>
@@ -46842,7 +46842,7 @@
       </c>
     </row>
     <row r="309" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A309" s="48"/>
+      <c r="A309" s="47"/>
       <c r="B309" s="13">
         <v>25</v>
       </c>
@@ -46972,7 +46972,7 @@
       </c>
     </row>
     <row r="310" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A310" s="48"/>
+      <c r="A310" s="47"/>
       <c r="B310" s="13">
         <v>26</v>
       </c>
@@ -47102,7 +47102,7 @@
       </c>
     </row>
     <row r="311" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A311" s="48"/>
+      <c r="A311" s="47"/>
       <c r="B311" s="13">
         <v>27</v>
       </c>
@@ -47232,7 +47232,7 @@
       </c>
     </row>
     <row r="312" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A312" s="48"/>
+      <c r="A312" s="47"/>
       <c r="B312" s="13">
         <v>28</v>
       </c>
@@ -47362,7 +47362,7 @@
       </c>
     </row>
     <row r="313" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A313" s="48"/>
+      <c r="A313" s="47"/>
       <c r="B313" s="13">
         <v>29</v>
       </c>
@@ -47492,7 +47492,7 @@
       </c>
     </row>
     <row r="314" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A314" s="48"/>
+      <c r="A314" s="47"/>
       <c r="B314" s="13">
         <v>30</v>
       </c>
@@ -47622,7 +47622,7 @@
       </c>
     </row>
     <row r="315" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A315" s="48"/>
+      <c r="A315" s="47"/>
       <c r="B315" s="13">
         <v>31</v>
       </c>
@@ -47752,7 +47752,7 @@
       </c>
     </row>
     <row r="316" spans="1:373" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A316" s="48"/>
+      <c r="A316" s="47"/>
       <c r="B316" s="16">
         <v>32</v>
       </c>
@@ -48211,7 +48211,7 @@
       <c r="NI316" s="2"/>
     </row>
     <row r="317" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A317" s="48"/>
+      <c r="A317" s="47"/>
       <c r="B317" s="13">
         <v>33</v>
       </c>
@@ -48340,7 +48340,7 @@
       </c>
     </row>
     <row r="318" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A318" s="48"/>
+      <c r="A318" s="47"/>
       <c r="B318" s="13">
         <v>34</v>
       </c>
@@ -48348,7 +48348,7 @@
         <v>54</v>
       </c>
       <c r="D318" s="3">
-        <v>0.55000000000000004</v>
+        <v>0.7</v>
       </c>
       <c r="E318" s="4">
         <v>0</v>
@@ -48469,7 +48469,7 @@
       </c>
     </row>
     <row r="319" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A319" s="48"/>
+      <c r="A319" s="47"/>
       <c r="B319" s="13">
         <v>35</v>
       </c>
@@ -48598,7 +48598,7 @@
       </c>
     </row>
     <row r="320" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A320" s="48"/>
+      <c r="A320" s="47"/>
       <c r="B320" s="13">
         <v>36</v>
       </c>
@@ -48727,7 +48727,7 @@
       </c>
     </row>
     <row r="321" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A321" s="48"/>
+      <c r="A321" s="47"/>
       <c r="B321" s="13">
         <v>37</v>
       </c>
@@ -48856,7 +48856,7 @@
       </c>
     </row>
     <row r="322" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A322" s="48"/>
+      <c r="A322" s="47"/>
       <c r="B322" s="13">
         <v>38</v>
       </c>
@@ -48985,7 +48985,7 @@
       </c>
     </row>
     <row r="323" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A323" s="48"/>
+      <c r="A323" s="47"/>
       <c r="B323" s="13">
         <v>39</v>
       </c>
@@ -49114,7 +49114,7 @@
       </c>
     </row>
     <row r="324" spans="1:373" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A324" s="49"/>
+      <c r="A324" s="48"/>
       <c r="B324" s="20">
         <v>40</v>
       </c>
@@ -49243,7 +49243,7 @@
       </c>
     </row>
     <row r="325" spans="1:373" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A325" s="46">
+      <c r="A325" s="49">
         <v>9</v>
       </c>
       <c r="B325" s="13">
@@ -49705,7 +49705,7 @@
       <c r="NI325"/>
     </row>
     <row r="326" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A326" s="46"/>
+      <c r="A326" s="49"/>
       <c r="B326" s="13">
         <v>2</v>
       </c>
@@ -49835,7 +49835,7 @@
       </c>
     </row>
     <row r="327" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A327" s="46"/>
+      <c r="A327" s="49"/>
       <c r="B327" s="13">
         <v>3</v>
       </c>
@@ -49965,7 +49965,7 @@
       </c>
     </row>
     <row r="328" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A328" s="46"/>
+      <c r="A328" s="49"/>
       <c r="B328" s="13">
         <v>4</v>
       </c>
@@ -50095,7 +50095,7 @@
       </c>
     </row>
     <row r="329" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A329" s="46"/>
+      <c r="A329" s="49"/>
       <c r="B329" s="13">
         <v>5</v>
       </c>
@@ -50225,7 +50225,7 @@
       </c>
     </row>
     <row r="330" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A330" s="46"/>
+      <c r="A330" s="49"/>
       <c r="B330" s="13">
         <v>6</v>
       </c>
@@ -50355,7 +50355,7 @@
       </c>
     </row>
     <row r="331" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A331" s="46"/>
+      <c r="A331" s="49"/>
       <c r="B331" s="13">
         <v>7</v>
       </c>
@@ -50485,7 +50485,7 @@
       </c>
     </row>
     <row r="332" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A332" s="46"/>
+      <c r="A332" s="49"/>
       <c r="B332" s="13">
         <v>8</v>
       </c>
@@ -50615,7 +50615,7 @@
       </c>
     </row>
     <row r="333" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A333" s="46"/>
+      <c r="A333" s="49"/>
       <c r="B333" s="13">
         <v>9</v>
       </c>
@@ -50745,7 +50745,7 @@
       </c>
     </row>
     <row r="334" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A334" s="46"/>
+      <c r="A334" s="49"/>
       <c r="B334" s="13">
         <v>10</v>
       </c>
@@ -50875,7 +50875,7 @@
       </c>
     </row>
     <row r="335" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A335" s="46"/>
+      <c r="A335" s="49"/>
       <c r="B335" s="13">
         <v>11</v>
       </c>
@@ -51005,7 +51005,7 @@
       </c>
     </row>
     <row r="336" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A336" s="46"/>
+      <c r="A336" s="49"/>
       <c r="B336" s="13">
         <v>12</v>
       </c>
@@ -51135,7 +51135,7 @@
       </c>
     </row>
     <row r="337" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A337" s="46"/>
+      <c r="A337" s="49"/>
       <c r="B337" s="13">
         <v>13</v>
       </c>
@@ -51265,7 +51265,7 @@
       </c>
     </row>
     <row r="338" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A338" s="46"/>
+      <c r="A338" s="49"/>
       <c r="B338" s="13">
         <v>14</v>
       </c>
@@ -51395,7 +51395,7 @@
       </c>
     </row>
     <row r="339" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A339" s="46"/>
+      <c r="A339" s="49"/>
       <c r="B339" s="13">
         <v>15</v>
       </c>
@@ -51525,7 +51525,7 @@
       </c>
     </row>
     <row r="340" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A340" s="46"/>
+      <c r="A340" s="49"/>
       <c r="B340" s="13">
         <v>16</v>
       </c>
@@ -51655,7 +51655,7 @@
       </c>
     </row>
     <row r="341" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A341" s="46"/>
+      <c r="A341" s="49"/>
       <c r="B341" s="13">
         <v>17</v>
       </c>
@@ -51785,7 +51785,7 @@
       </c>
     </row>
     <row r="342" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A342" s="46"/>
+      <c r="A342" s="49"/>
       <c r="B342" s="13">
         <v>18</v>
       </c>
@@ -51915,7 +51915,7 @@
       </c>
     </row>
     <row r="343" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A343" s="46"/>
+      <c r="A343" s="49"/>
       <c r="B343" s="13">
         <v>19</v>
       </c>
@@ -52045,7 +52045,7 @@
       </c>
     </row>
     <row r="344" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A344" s="46"/>
+      <c r="A344" s="49"/>
       <c r="B344" s="13">
         <v>20</v>
       </c>
@@ -52175,7 +52175,7 @@
       </c>
     </row>
     <row r="345" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A345" s="46"/>
+      <c r="A345" s="49"/>
       <c r="B345" s="13">
         <v>21</v>
       </c>
@@ -52305,7 +52305,7 @@
       </c>
     </row>
     <row r="346" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A346" s="46"/>
+      <c r="A346" s="49"/>
       <c r="B346" s="13">
         <v>22</v>
       </c>
@@ -52435,7 +52435,7 @@
       </c>
     </row>
     <row r="347" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A347" s="46"/>
+      <c r="A347" s="49"/>
       <c r="B347" s="13">
         <v>23</v>
       </c>
@@ -52565,7 +52565,7 @@
       </c>
     </row>
     <row r="348" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A348" s="46"/>
+      <c r="A348" s="49"/>
       <c r="B348" s="13">
         <v>24</v>
       </c>
@@ -52695,7 +52695,7 @@
       </c>
     </row>
     <row r="349" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A349" s="46"/>
+      <c r="A349" s="49"/>
       <c r="B349" s="13">
         <v>25</v>
       </c>
@@ -52825,7 +52825,7 @@
       </c>
     </row>
     <row r="350" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A350" s="46"/>
+      <c r="A350" s="49"/>
       <c r="B350" s="13">
         <v>26</v>
       </c>
@@ -52955,7 +52955,7 @@
       </c>
     </row>
     <row r="351" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A351" s="46"/>
+      <c r="A351" s="49"/>
       <c r="B351" s="13">
         <v>27</v>
       </c>
@@ -53085,7 +53085,7 @@
       </c>
     </row>
     <row r="352" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A352" s="46"/>
+      <c r="A352" s="49"/>
       <c r="B352" s="13">
         <v>28</v>
       </c>
@@ -53215,7 +53215,7 @@
       </c>
     </row>
     <row r="353" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A353" s="46"/>
+      <c r="A353" s="49"/>
       <c r="B353" s="13">
         <v>29</v>
       </c>
@@ -53345,7 +53345,7 @@
       </c>
     </row>
     <row r="354" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A354" s="46"/>
+      <c r="A354" s="49"/>
       <c r="B354" s="13">
         <v>30</v>
       </c>
@@ -53475,7 +53475,7 @@
       </c>
     </row>
     <row r="355" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A355" s="46"/>
+      <c r="A355" s="49"/>
       <c r="B355" s="13">
         <v>31</v>
       </c>
@@ -53605,7 +53605,7 @@
       </c>
     </row>
     <row r="356" spans="1:373" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A356" s="46"/>
+      <c r="A356" s="49"/>
       <c r="B356" s="16">
         <v>32</v>
       </c>
@@ -54064,7 +54064,7 @@
       <c r="NI356" s="2"/>
     </row>
     <row r="357" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A357" s="46"/>
+      <c r="A357" s="49"/>
       <c r="B357" s="13">
         <v>33</v>
       </c>
@@ -54193,7 +54193,7 @@
       </c>
     </row>
     <row r="358" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A358" s="46"/>
+      <c r="A358" s="49"/>
       <c r="B358" s="13">
         <v>34</v>
       </c>
@@ -54201,7 +54201,7 @@
         <v>54</v>
       </c>
       <c r="D358" s="3">
-        <v>0.55000000000000004</v>
+        <v>0.7</v>
       </c>
       <c r="E358" s="4">
         <v>0</v>
@@ -54322,7 +54322,7 @@
       </c>
     </row>
     <row r="359" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A359" s="46"/>
+      <c r="A359" s="49"/>
       <c r="B359" s="13">
         <v>35</v>
       </c>
@@ -54451,7 +54451,7 @@
       </c>
     </row>
     <row r="360" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A360" s="46"/>
+      <c r="A360" s="49"/>
       <c r="B360" s="13">
         <v>36</v>
       </c>
@@ -54580,7 +54580,7 @@
       </c>
     </row>
     <row r="361" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A361" s="46"/>
+      <c r="A361" s="49"/>
       <c r="B361" s="13">
         <v>37</v>
       </c>
@@ -54709,7 +54709,7 @@
       </c>
     </row>
     <row r="362" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A362" s="46"/>
+      <c r="A362" s="49"/>
       <c r="B362" s="13">
         <v>38</v>
       </c>
@@ -54838,7 +54838,7 @@
       </c>
     </row>
     <row r="363" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A363" s="46"/>
+      <c r="A363" s="49"/>
       <c r="B363" s="13">
         <v>39</v>
       </c>
@@ -54967,7 +54967,7 @@
       </c>
     </row>
     <row r="364" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A364" s="46"/>
+      <c r="A364" s="49"/>
       <c r="B364" s="13">
         <v>40</v>
       </c>
@@ -55096,7 +55096,7 @@
       </c>
     </row>
     <row r="365" spans="1:373" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A365" s="47">
+      <c r="A365" s="46">
         <v>10</v>
       </c>
       <c r="B365" s="16">
@@ -55558,7 +55558,7 @@
       <c r="NI365"/>
     </row>
     <row r="366" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A366" s="48"/>
+      <c r="A366" s="47"/>
       <c r="B366" s="13">
         <v>2</v>
       </c>
@@ -55688,7 +55688,7 @@
       </c>
     </row>
     <row r="367" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A367" s="48"/>
+      <c r="A367" s="47"/>
       <c r="B367" s="13">
         <v>3</v>
       </c>
@@ -55818,7 +55818,7 @@
       </c>
     </row>
     <row r="368" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A368" s="48"/>
+      <c r="A368" s="47"/>
       <c r="B368" s="13">
         <v>4</v>
       </c>
@@ -55948,7 +55948,7 @@
       </c>
     </row>
     <row r="369" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A369" s="48"/>
+      <c r="A369" s="47"/>
       <c r="B369" s="13">
         <v>5</v>
       </c>
@@ -56078,7 +56078,7 @@
       </c>
     </row>
     <row r="370" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A370" s="48"/>
+      <c r="A370" s="47"/>
       <c r="B370" s="13">
         <v>6</v>
       </c>
@@ -56208,7 +56208,7 @@
       </c>
     </row>
     <row r="371" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A371" s="48"/>
+      <c r="A371" s="47"/>
       <c r="B371" s="13">
         <v>7</v>
       </c>
@@ -56338,7 +56338,7 @@
       </c>
     </row>
     <row r="372" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A372" s="48"/>
+      <c r="A372" s="47"/>
       <c r="B372" s="13">
         <v>8</v>
       </c>
@@ -56468,7 +56468,7 @@
       </c>
     </row>
     <row r="373" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A373" s="48"/>
+      <c r="A373" s="47"/>
       <c r="B373" s="13">
         <v>9</v>
       </c>
@@ -56598,7 +56598,7 @@
       </c>
     </row>
     <row r="374" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A374" s="48"/>
+      <c r="A374" s="47"/>
       <c r="B374" s="13">
         <v>10</v>
       </c>
@@ -56728,7 +56728,7 @@
       </c>
     </row>
     <row r="375" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A375" s="48"/>
+      <c r="A375" s="47"/>
       <c r="B375" s="13">
         <v>11</v>
       </c>
@@ -56858,7 +56858,7 @@
       </c>
     </row>
     <row r="376" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A376" s="48"/>
+      <c r="A376" s="47"/>
       <c r="B376" s="13">
         <v>12</v>
       </c>
@@ -56988,7 +56988,7 @@
       </c>
     </row>
     <row r="377" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A377" s="48"/>
+      <c r="A377" s="47"/>
       <c r="B377" s="13">
         <v>13</v>
       </c>
@@ -57118,7 +57118,7 @@
       </c>
     </row>
     <row r="378" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A378" s="48"/>
+      <c r="A378" s="47"/>
       <c r="B378" s="13">
         <v>14</v>
       </c>
@@ -57248,7 +57248,7 @@
       </c>
     </row>
     <row r="379" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A379" s="48"/>
+      <c r="A379" s="47"/>
       <c r="B379" s="13">
         <v>15</v>
       </c>
@@ -57378,7 +57378,7 @@
       </c>
     </row>
     <row r="380" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A380" s="48"/>
+      <c r="A380" s="47"/>
       <c r="B380" s="13">
         <v>16</v>
       </c>
@@ -57508,7 +57508,7 @@
       </c>
     </row>
     <row r="381" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A381" s="48"/>
+      <c r="A381" s="47"/>
       <c r="B381" s="13">
         <v>17</v>
       </c>
@@ -57638,7 +57638,7 @@
       </c>
     </row>
     <row r="382" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A382" s="48"/>
+      <c r="A382" s="47"/>
       <c r="B382" s="13">
         <v>18</v>
       </c>
@@ -57768,7 +57768,7 @@
       </c>
     </row>
     <row r="383" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A383" s="48"/>
+      <c r="A383" s="47"/>
       <c r="B383" s="13">
         <v>19</v>
       </c>
@@ -57898,7 +57898,7 @@
       </c>
     </row>
     <row r="384" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A384" s="48"/>
+      <c r="A384" s="47"/>
       <c r="B384" s="13">
         <v>20</v>
       </c>
@@ -58028,7 +58028,7 @@
       </c>
     </row>
     <row r="385" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A385" s="48"/>
+      <c r="A385" s="47"/>
       <c r="B385" s="13">
         <v>21</v>
       </c>
@@ -58158,7 +58158,7 @@
       </c>
     </row>
     <row r="386" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A386" s="48"/>
+      <c r="A386" s="47"/>
       <c r="B386" s="13">
         <v>22</v>
       </c>
@@ -58288,7 +58288,7 @@
       </c>
     </row>
     <row r="387" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A387" s="48"/>
+      <c r="A387" s="47"/>
       <c r="B387" s="13">
         <v>23</v>
       </c>
@@ -58418,7 +58418,7 @@
       </c>
     </row>
     <row r="388" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A388" s="48"/>
+      <c r="A388" s="47"/>
       <c r="B388" s="13">
         <v>24</v>
       </c>
@@ -58548,7 +58548,7 @@
       </c>
     </row>
     <row r="389" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A389" s="48"/>
+      <c r="A389" s="47"/>
       <c r="B389" s="13">
         <v>25</v>
       </c>
@@ -58678,7 +58678,7 @@
       </c>
     </row>
     <row r="390" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A390" s="48"/>
+      <c r="A390" s="47"/>
       <c r="B390" s="13">
         <v>26</v>
       </c>
@@ -58808,7 +58808,7 @@
       </c>
     </row>
     <row r="391" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A391" s="48"/>
+      <c r="A391" s="47"/>
       <c r="B391" s="13">
         <v>27</v>
       </c>
@@ -58938,7 +58938,7 @@
       </c>
     </row>
     <row r="392" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A392" s="48"/>
+      <c r="A392" s="47"/>
       <c r="B392" s="13">
         <v>28</v>
       </c>
@@ -59068,7 +59068,7 @@
       </c>
     </row>
     <row r="393" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A393" s="48"/>
+      <c r="A393" s="47"/>
       <c r="B393" s="13">
         <v>29</v>
       </c>
@@ -59198,7 +59198,7 @@
       </c>
     </row>
     <row r="394" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A394" s="48"/>
+      <c r="A394" s="47"/>
       <c r="B394" s="13">
         <v>30</v>
       </c>
@@ -59328,7 +59328,7 @@
       </c>
     </row>
     <row r="395" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A395" s="48"/>
+      <c r="A395" s="47"/>
       <c r="B395" s="13">
         <v>31</v>
       </c>
@@ -59458,7 +59458,7 @@
       </c>
     </row>
     <row r="396" spans="1:373" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A396" s="48"/>
+      <c r="A396" s="47"/>
       <c r="B396" s="16">
         <v>32</v>
       </c>
@@ -59917,7 +59917,7 @@
       <c r="NI396" s="2"/>
     </row>
     <row r="397" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A397" s="48"/>
+      <c r="A397" s="47"/>
       <c r="B397" s="13">
         <v>33</v>
       </c>
@@ -60046,7 +60046,7 @@
       </c>
     </row>
     <row r="398" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A398" s="48"/>
+      <c r="A398" s="47"/>
       <c r="B398" s="13">
         <v>34</v>
       </c>
@@ -60054,7 +60054,7 @@
         <v>54</v>
       </c>
       <c r="D398" s="3">
-        <v>0.5</v>
+        <v>0.65</v>
       </c>
       <c r="E398" s="4">
         <v>0</v>
@@ -60175,7 +60175,7 @@
       </c>
     </row>
     <row r="399" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A399" s="48"/>
+      <c r="A399" s="47"/>
       <c r="B399" s="13">
         <v>35</v>
       </c>
@@ -60304,7 +60304,7 @@
       </c>
     </row>
     <row r="400" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A400" s="48"/>
+      <c r="A400" s="47"/>
       <c r="B400" s="13">
         <v>36</v>
       </c>
@@ -60433,7 +60433,7 @@
       </c>
     </row>
     <row r="401" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A401" s="48"/>
+      <c r="A401" s="47"/>
       <c r="B401" s="13">
         <v>37</v>
       </c>
@@ -60562,7 +60562,7 @@
       </c>
     </row>
     <row r="402" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A402" s="48"/>
+      <c r="A402" s="47"/>
       <c r="B402" s="13">
         <v>38</v>
       </c>
@@ -60691,7 +60691,7 @@
       </c>
     </row>
     <row r="403" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A403" s="48"/>
+      <c r="A403" s="47"/>
       <c r="B403" s="13">
         <v>39</v>
       </c>
@@ -60820,7 +60820,7 @@
       </c>
     </row>
     <row r="404" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A404" s="49"/>
+      <c r="A404" s="48"/>
       <c r="B404" s="20">
         <v>40</v>
       </c>
@@ -60949,7 +60949,7 @@
       </c>
     </row>
     <row r="405" spans="1:373" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A405" s="46">
+      <c r="A405" s="49">
         <v>11</v>
       </c>
       <c r="B405" s="13">
@@ -61411,7 +61411,7 @@
       <c r="NI405"/>
     </row>
     <row r="406" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A406" s="46"/>
+      <c r="A406" s="49"/>
       <c r="B406" s="13">
         <v>2</v>
       </c>
@@ -61541,7 +61541,7 @@
       </c>
     </row>
     <row r="407" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A407" s="46"/>
+      <c r="A407" s="49"/>
       <c r="B407" s="13">
         <v>3</v>
       </c>
@@ -61671,7 +61671,7 @@
       </c>
     </row>
     <row r="408" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A408" s="46"/>
+      <c r="A408" s="49"/>
       <c r="B408" s="13">
         <v>4</v>
       </c>
@@ -61801,7 +61801,7 @@
       </c>
     </row>
     <row r="409" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A409" s="46"/>
+      <c r="A409" s="49"/>
       <c r="B409" s="13">
         <v>5</v>
       </c>
@@ -61931,7 +61931,7 @@
       </c>
     </row>
     <row r="410" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A410" s="46"/>
+      <c r="A410" s="49"/>
       <c r="B410" s="13">
         <v>6</v>
       </c>
@@ -62061,7 +62061,7 @@
       </c>
     </row>
     <row r="411" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A411" s="46"/>
+      <c r="A411" s="49"/>
       <c r="B411" s="13">
         <v>7</v>
       </c>
@@ -62191,7 +62191,7 @@
       </c>
     </row>
     <row r="412" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A412" s="46"/>
+      <c r="A412" s="49"/>
       <c r="B412" s="13">
         <v>8</v>
       </c>
@@ -62321,7 +62321,7 @@
       </c>
     </row>
     <row r="413" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A413" s="46"/>
+      <c r="A413" s="49"/>
       <c r="B413" s="13">
         <v>9</v>
       </c>
@@ -62451,7 +62451,7 @@
       </c>
     </row>
     <row r="414" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A414" s="46"/>
+      <c r="A414" s="49"/>
       <c r="B414" s="13">
         <v>10</v>
       </c>
@@ -62581,7 +62581,7 @@
       </c>
     </row>
     <row r="415" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A415" s="46"/>
+      <c r="A415" s="49"/>
       <c r="B415" s="13">
         <v>11</v>
       </c>
@@ -62711,7 +62711,7 @@
       </c>
     </row>
     <row r="416" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A416" s="46"/>
+      <c r="A416" s="49"/>
       <c r="B416" s="13">
         <v>12</v>
       </c>
@@ -62841,7 +62841,7 @@
       </c>
     </row>
     <row r="417" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A417" s="46"/>
+      <c r="A417" s="49"/>
       <c r="B417" s="13">
         <v>13</v>
       </c>
@@ -62971,7 +62971,7 @@
       </c>
     </row>
     <row r="418" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A418" s="46"/>
+      <c r="A418" s="49"/>
       <c r="B418" s="13">
         <v>14</v>
       </c>
@@ -63101,7 +63101,7 @@
       </c>
     </row>
     <row r="419" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A419" s="46"/>
+      <c r="A419" s="49"/>
       <c r="B419" s="13">
         <v>15</v>
       </c>
@@ -63231,7 +63231,7 @@
       </c>
     </row>
     <row r="420" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A420" s="46"/>
+      <c r="A420" s="49"/>
       <c r="B420" s="13">
         <v>16</v>
       </c>
@@ -63361,7 +63361,7 @@
       </c>
     </row>
     <row r="421" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A421" s="46"/>
+      <c r="A421" s="49"/>
       <c r="B421" s="13">
         <v>17</v>
       </c>
@@ -63491,7 +63491,7 @@
       </c>
     </row>
     <row r="422" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A422" s="46"/>
+      <c r="A422" s="49"/>
       <c r="B422" s="13">
         <v>18</v>
       </c>
@@ -63621,7 +63621,7 @@
       </c>
     </row>
     <row r="423" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A423" s="46"/>
+      <c r="A423" s="49"/>
       <c r="B423" s="13">
         <v>19</v>
       </c>
@@ -63751,7 +63751,7 @@
       </c>
     </row>
     <row r="424" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A424" s="46"/>
+      <c r="A424" s="49"/>
       <c r="B424" s="13">
         <v>20</v>
       </c>
@@ -63881,7 +63881,7 @@
       </c>
     </row>
     <row r="425" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A425" s="46"/>
+      <c r="A425" s="49"/>
       <c r="B425" s="13">
         <v>21</v>
       </c>
@@ -64011,7 +64011,7 @@
       </c>
     </row>
     <row r="426" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A426" s="46"/>
+      <c r="A426" s="49"/>
       <c r="B426" s="13">
         <v>22</v>
       </c>
@@ -64141,7 +64141,7 @@
       </c>
     </row>
     <row r="427" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A427" s="46"/>
+      <c r="A427" s="49"/>
       <c r="B427" s="13">
         <v>23</v>
       </c>
@@ -64271,7 +64271,7 @@
       </c>
     </row>
     <row r="428" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A428" s="46"/>
+      <c r="A428" s="49"/>
       <c r="B428" s="13">
         <v>24</v>
       </c>
@@ -64401,7 +64401,7 @@
       </c>
     </row>
     <row r="429" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A429" s="46"/>
+      <c r="A429" s="49"/>
       <c r="B429" s="13">
         <v>25</v>
       </c>
@@ -64531,7 +64531,7 @@
       </c>
     </row>
     <row r="430" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A430" s="46"/>
+      <c r="A430" s="49"/>
       <c r="B430" s="13">
         <v>26</v>
       </c>
@@ -64661,7 +64661,7 @@
       </c>
     </row>
     <row r="431" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A431" s="46"/>
+      <c r="A431" s="49"/>
       <c r="B431" s="13">
         <v>27</v>
       </c>
@@ -64791,7 +64791,7 @@
       </c>
     </row>
     <row r="432" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A432" s="46"/>
+      <c r="A432" s="49"/>
       <c r="B432" s="13">
         <v>28</v>
       </c>
@@ -64921,7 +64921,7 @@
       </c>
     </row>
     <row r="433" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A433" s="46"/>
+      <c r="A433" s="49"/>
       <c r="B433" s="13">
         <v>29</v>
       </c>
@@ -65051,7 +65051,7 @@
       </c>
     </row>
     <row r="434" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A434" s="46"/>
+      <c r="A434" s="49"/>
       <c r="B434" s="13">
         <v>30</v>
       </c>
@@ -65181,7 +65181,7 @@
       </c>
     </row>
     <row r="435" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A435" s="46"/>
+      <c r="A435" s="49"/>
       <c r="B435" s="13">
         <v>31</v>
       </c>
@@ -65311,7 +65311,7 @@
       </c>
     </row>
     <row r="436" spans="1:373" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A436" s="46"/>
+      <c r="A436" s="49"/>
       <c r="B436" s="16">
         <v>32</v>
       </c>
@@ -65770,7 +65770,7 @@
       <c r="NI436" s="2"/>
     </row>
     <row r="437" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A437" s="46"/>
+      <c r="A437" s="49"/>
       <c r="B437" s="13">
         <v>33</v>
       </c>
@@ -65899,7 +65899,7 @@
       </c>
     </row>
     <row r="438" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A438" s="46"/>
+      <c r="A438" s="49"/>
       <c r="B438" s="13">
         <v>34</v>
       </c>
@@ -65907,7 +65907,7 @@
         <v>54</v>
       </c>
       <c r="D438" s="3">
-        <v>0.5</v>
+        <v>0.65</v>
       </c>
       <c r="E438" s="4">
         <v>0</v>
@@ -66028,7 +66028,7 @@
       </c>
     </row>
     <row r="439" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A439" s="46"/>
+      <c r="A439" s="49"/>
       <c r="B439" s="13">
         <v>35</v>
       </c>
@@ -66157,7 +66157,7 @@
       </c>
     </row>
     <row r="440" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A440" s="46"/>
+      <c r="A440" s="49"/>
       <c r="B440" s="13">
         <v>36</v>
       </c>
@@ -66286,7 +66286,7 @@
       </c>
     </row>
     <row r="441" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A441" s="46"/>
+      <c r="A441" s="49"/>
       <c r="B441" s="13">
         <v>37</v>
       </c>
@@ -66415,7 +66415,7 @@
       </c>
     </row>
     <row r="442" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A442" s="46"/>
+      <c r="A442" s="49"/>
       <c r="B442" s="13">
         <v>38</v>
       </c>
@@ -66544,7 +66544,7 @@
       </c>
     </row>
     <row r="443" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A443" s="46"/>
+      <c r="A443" s="49"/>
       <c r="B443" s="13">
         <v>39</v>
       </c>
@@ -66673,7 +66673,7 @@
       </c>
     </row>
     <row r="444" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A444" s="46"/>
+      <c r="A444" s="49"/>
       <c r="B444" s="13">
         <v>40</v>
       </c>
@@ -66802,7 +66802,7 @@
       </c>
     </row>
     <row r="445" spans="1:373" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A445" s="47">
+      <c r="A445" s="46">
         <v>12</v>
       </c>
       <c r="B445" s="16">
@@ -67264,7 +67264,7 @@
       <c r="NI445"/>
     </row>
     <row r="446" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A446" s="48"/>
+      <c r="A446" s="47"/>
       <c r="B446" s="13">
         <v>2</v>
       </c>
@@ -67394,7 +67394,7 @@
       </c>
     </row>
     <row r="447" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A447" s="48"/>
+      <c r="A447" s="47"/>
       <c r="B447" s="13">
         <v>3</v>
       </c>
@@ -67524,7 +67524,7 @@
       </c>
     </row>
     <row r="448" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A448" s="48"/>
+      <c r="A448" s="47"/>
       <c r="B448" s="13">
         <v>4</v>
       </c>
@@ -67654,7 +67654,7 @@
       </c>
     </row>
     <row r="449" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A449" s="48"/>
+      <c r="A449" s="47"/>
       <c r="B449" s="13">
         <v>5</v>
       </c>
@@ -67784,7 +67784,7 @@
       </c>
     </row>
     <row r="450" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A450" s="48"/>
+      <c r="A450" s="47"/>
       <c r="B450" s="13">
         <v>6</v>
       </c>
@@ -67914,7 +67914,7 @@
       </c>
     </row>
     <row r="451" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A451" s="48"/>
+      <c r="A451" s="47"/>
       <c r="B451" s="13">
         <v>7</v>
       </c>
@@ -68044,7 +68044,7 @@
       </c>
     </row>
     <row r="452" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A452" s="48"/>
+      <c r="A452" s="47"/>
       <c r="B452" s="13">
         <v>8</v>
       </c>
@@ -68174,7 +68174,7 @@
       </c>
     </row>
     <row r="453" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A453" s="48"/>
+      <c r="A453" s="47"/>
       <c r="B453" s="13">
         <v>9</v>
       </c>
@@ -68304,7 +68304,7 @@
       </c>
     </row>
     <row r="454" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A454" s="48"/>
+      <c r="A454" s="47"/>
       <c r="B454" s="13">
         <v>10</v>
       </c>
@@ -68434,7 +68434,7 @@
       </c>
     </row>
     <row r="455" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A455" s="48"/>
+      <c r="A455" s="47"/>
       <c r="B455" s="13">
         <v>11</v>
       </c>
@@ -68564,7 +68564,7 @@
       </c>
     </row>
     <row r="456" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A456" s="48"/>
+      <c r="A456" s="47"/>
       <c r="B456" s="13">
         <v>12</v>
       </c>
@@ -68694,7 +68694,7 @@
       </c>
     </row>
     <row r="457" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A457" s="48"/>
+      <c r="A457" s="47"/>
       <c r="B457" s="13">
         <v>13</v>
       </c>
@@ -68824,7 +68824,7 @@
       </c>
     </row>
     <row r="458" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A458" s="48"/>
+      <c r="A458" s="47"/>
       <c r="B458" s="13">
         <v>14</v>
       </c>
@@ -68954,7 +68954,7 @@
       </c>
     </row>
     <row r="459" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A459" s="48"/>
+      <c r="A459" s="47"/>
       <c r="B459" s="13">
         <v>15</v>
       </c>
@@ -69084,7 +69084,7 @@
       </c>
     </row>
     <row r="460" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A460" s="48"/>
+      <c r="A460" s="47"/>
       <c r="B460" s="13">
         <v>16</v>
       </c>
@@ -69214,7 +69214,7 @@
       </c>
     </row>
     <row r="461" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A461" s="48"/>
+      <c r="A461" s="47"/>
       <c r="B461" s="13">
         <v>17</v>
       </c>
@@ -69344,7 +69344,7 @@
       </c>
     </row>
     <row r="462" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A462" s="48"/>
+      <c r="A462" s="47"/>
       <c r="B462" s="13">
         <v>18</v>
       </c>
@@ -69474,7 +69474,7 @@
       </c>
     </row>
     <row r="463" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A463" s="48"/>
+      <c r="A463" s="47"/>
       <c r="B463" s="13">
         <v>19</v>
       </c>
@@ -69604,7 +69604,7 @@
       </c>
     </row>
     <row r="464" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A464" s="48"/>
+      <c r="A464" s="47"/>
       <c r="B464" s="13">
         <v>20</v>
       </c>
@@ -69734,7 +69734,7 @@
       </c>
     </row>
     <row r="465" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A465" s="48"/>
+      <c r="A465" s="47"/>
       <c r="B465" s="13">
         <v>21</v>
       </c>
@@ -69864,7 +69864,7 @@
       </c>
     </row>
     <row r="466" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A466" s="48"/>
+      <c r="A466" s="47"/>
       <c r="B466" s="13">
         <v>22</v>
       </c>
@@ -69994,7 +69994,7 @@
       </c>
     </row>
     <row r="467" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A467" s="48"/>
+      <c r="A467" s="47"/>
       <c r="B467" s="13">
         <v>23</v>
       </c>
@@ -70124,7 +70124,7 @@
       </c>
     </row>
     <row r="468" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A468" s="48"/>
+      <c r="A468" s="47"/>
       <c r="B468" s="13">
         <v>24</v>
       </c>
@@ -70254,7 +70254,7 @@
       </c>
     </row>
     <row r="469" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A469" s="48"/>
+      <c r="A469" s="47"/>
       <c r="B469" s="13">
         <v>25</v>
       </c>
@@ -70384,7 +70384,7 @@
       </c>
     </row>
     <row r="470" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A470" s="48"/>
+      <c r="A470" s="47"/>
       <c r="B470" s="13">
         <v>26</v>
       </c>
@@ -70514,7 +70514,7 @@
       </c>
     </row>
     <row r="471" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A471" s="48"/>
+      <c r="A471" s="47"/>
       <c r="B471" s="13">
         <v>27</v>
       </c>
@@ -70644,7 +70644,7 @@
       </c>
     </row>
     <row r="472" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A472" s="48"/>
+      <c r="A472" s="47"/>
       <c r="B472" s="13">
         <v>28</v>
       </c>
@@ -70774,7 +70774,7 @@
       </c>
     </row>
     <row r="473" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A473" s="48"/>
+      <c r="A473" s="47"/>
       <c r="B473" s="13">
         <v>29</v>
       </c>
@@ -70904,7 +70904,7 @@
       </c>
     </row>
     <row r="474" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A474" s="48"/>
+      <c r="A474" s="47"/>
       <c r="B474" s="13">
         <v>30</v>
       </c>
@@ -71034,7 +71034,7 @@
       </c>
     </row>
     <row r="475" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A475" s="48"/>
+      <c r="A475" s="47"/>
       <c r="B475" s="13">
         <v>31</v>
       </c>
@@ -71164,7 +71164,7 @@
       </c>
     </row>
     <row r="476" spans="1:373" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A476" s="48"/>
+      <c r="A476" s="47"/>
       <c r="B476" s="16">
         <v>32</v>
       </c>
@@ -71623,7 +71623,7 @@
       <c r="NI476" s="2"/>
     </row>
     <row r="477" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A477" s="48"/>
+      <c r="A477" s="47"/>
       <c r="B477" s="13">
         <v>33</v>
       </c>
@@ -71752,7 +71752,7 @@
       </c>
     </row>
     <row r="478" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A478" s="48"/>
+      <c r="A478" s="47"/>
       <c r="B478" s="13">
         <v>34</v>
       </c>
@@ -71760,7 +71760,7 @@
         <v>54</v>
       </c>
       <c r="D478" s="3">
-        <v>0.5</v>
+        <v>0.65</v>
       </c>
       <c r="E478" s="4">
         <v>0</v>
@@ -71881,7 +71881,7 @@
       </c>
     </row>
     <row r="479" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A479" s="48"/>
+      <c r="A479" s="47"/>
       <c r="B479" s="13">
         <v>35</v>
       </c>
@@ -72010,7 +72010,7 @@
       </c>
     </row>
     <row r="480" spans="1:373" x14ac:dyDescent="0.2">
-      <c r="A480" s="48"/>
+      <c r="A480" s="47"/>
       <c r="B480" s="13">
         <v>36</v>
       </c>
@@ -72139,7 +72139,7 @@
       </c>
     </row>
     <row r="481" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A481" s="48"/>
+      <c r="A481" s="47"/>
       <c r="B481" s="13">
         <v>37</v>
       </c>
@@ -72268,7 +72268,7 @@
       </c>
     </row>
     <row r="482" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A482" s="48"/>
+      <c r="A482" s="47"/>
       <c r="B482" s="13">
         <v>38</v>
       </c>
@@ -72397,7 +72397,7 @@
       </c>
     </row>
     <row r="483" spans="1:43" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A483" s="48"/>
+      <c r="A483" s="47"/>
       <c r="B483" s="13">
         <v>39</v>
       </c>
@@ -72526,7 +72526,7 @@
       </c>
     </row>
     <row r="484" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A484" s="49"/>
+      <c r="A484" s="48"/>
       <c r="B484" s="20">
         <v>40</v>
       </c>
@@ -72760,23 +72760,23 @@
     <row r="588" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A205:A244"/>
+    <mergeCell ref="A245:A284"/>
+    <mergeCell ref="A5:A44"/>
+    <mergeCell ref="A45:A84"/>
+    <mergeCell ref="A85:A124"/>
+    <mergeCell ref="A125:A164"/>
+    <mergeCell ref="A165:A204"/>
+    <mergeCell ref="AI1:AQ1"/>
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="B1:B4"/>
+    <mergeCell ref="C1:C4"/>
+    <mergeCell ref="D1:AH1"/>
     <mergeCell ref="A285:A324"/>
     <mergeCell ref="A325:A364"/>
     <mergeCell ref="A365:A404"/>
     <mergeCell ref="A405:A444"/>
     <mergeCell ref="A445:A484"/>
-    <mergeCell ref="AI1:AQ1"/>
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="B1:B4"/>
-    <mergeCell ref="C1:C4"/>
-    <mergeCell ref="D1:AH1"/>
-    <mergeCell ref="A5:A44"/>
-    <mergeCell ref="A45:A84"/>
-    <mergeCell ref="A85:A124"/>
-    <mergeCell ref="A125:A164"/>
-    <mergeCell ref="A165:A204"/>
-    <mergeCell ref="A205:A244"/>
-    <mergeCell ref="A245:A284"/>
   </mergeCells>
   <conditionalFormatting sqref="AI2:AQ2">
     <cfRule type="colorScale" priority="85">

</xml_diff>